<commit_message>
Modificaciones en ubicación de recursos
Modificaciones en ubicación de recursos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion09/ESCALETA FINAL CN_11_09_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion09/ESCALETA FINAL CN_11_09_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="60" windowWidth="20490" windowHeight="7695"/>
   </bookViews>
@@ -10,10 +15,13 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="DATOS" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$P$1:$P$93</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$P$1:$P$100</definedName>
   </definedNames>
-  <calcPr calcId="144525" iterateCount="2" iterateDelta="10"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="233">
   <si>
     <t>Asignatura</t>
   </si>
@@ -515,9 +523,6 @@
   </si>
   <si>
     <t>Actividades sobre La autoionización del agua</t>
-  </si>
-  <si>
-    <t>Recurso M101A-02</t>
   </si>
   <si>
     <t>FQ_10_07</t>
@@ -682,12 +687,6 @@
     <t>Recurso M101A-05</t>
   </si>
   <si>
-    <t>Competencias: preparación de un indicador ácido-base</t>
-  </si>
-  <si>
-    <t>Actividad que propone realizar un experimento para comprender la importancia de los indicadores ácido-base</t>
-  </si>
-  <si>
     <t>Actividad que propone realizar un experimento para determinar la concentración de una disolución mediante una valoración ácido-base</t>
   </si>
   <si>
@@ -752,13 +751,70 @@
   </si>
   <si>
     <t>Competencias: cantidad de hidrogenocarbonato en un antiácido</t>
+  </si>
+  <si>
+    <t>La autodisociación del agua</t>
+  </si>
+  <si>
+    <t>Secuencia de imágenes que permite explicar la propiedad del agua de actuar como ácido o base</t>
+  </si>
+  <si>
+    <t>Secuencia de imágenes</t>
+  </si>
+  <si>
+    <t>Recursos M aleatorios y diaporama F1</t>
+  </si>
+  <si>
+    <t>Diaporama F1-01</t>
+  </si>
+  <si>
+    <t>RM_01_02_CO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La medida de la acidez </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interactivo para explicar el concepto de pH y pOH en disoluciones </t>
+  </si>
+  <si>
+    <t>Recurso F6-02</t>
+  </si>
+  <si>
+    <t>Las sustancias indicadoras ácido-base</t>
+  </si>
+  <si>
+    <t>Interactivo que guía el proceso para elaborar en el laboratorio sustancias indicadoras ácido-base</t>
+  </si>
+  <si>
+    <t>Recurso F13B-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proyecto: análisis de un producto de cuidado personal </t>
+  </si>
+  <si>
+    <t>3º ESO</t>
+  </si>
+  <si>
+    <t>La industria química</t>
+  </si>
+  <si>
+    <t>Proyecto: análisis de un producto de higiene personal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El uso de los ácidos y bases </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interactivo que muestra las aplicaciones de diferentes ácidos y bases </t>
+  </si>
+  <si>
+    <t>Actividad que guía el trabajo colaborativo sobre la investigación de las cualidades del champú</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -802,8 +858,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -849,6 +912,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1143,7 +1224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1243,6 +1324,67 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1258,6 +1400,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Hoja1"/>
+      <sheetName val="DATOS"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1515,7 +1672,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1524,10 +1681,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:W93"/>
+  <dimension ref="A1:W100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="T44" sqref="T44"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P49" sqref="P49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1554,7 +1711,7 @@
     <col min="21" max="21" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
@@ -1617,7 +1774,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="12" customFormat="1" ht="29.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="48"/>
       <c r="B2" s="48"/>
       <c r="C2" s="48"/>
@@ -1644,7 +1801,7 @@
       <c r="T2" s="48"/>
       <c r="U2" s="48"/>
     </row>
-    <row r="3" spans="1:23" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>67</v>
       </c>
@@ -1657,27 +1814,51 @@
       <c r="D3" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="E3" s="25" t="s">
-        <v>100</v>
-      </c>
+      <c r="E3" s="25"/>
       <c r="F3" s="26"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="39"/>
+      <c r="G3" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="H3" s="30">
+        <v>1</v>
+      </c>
+      <c r="I3" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="K3" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="39" t="s">
+        <v>36</v>
+      </c>
       <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="4"/>
-    </row>
-    <row r="4" spans="1:23" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O3" s="38"/>
+      <c r="P3" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>6</v>
+      </c>
+      <c r="R3" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>67</v>
       </c>
@@ -1691,26 +1872,26 @@
         <v>92</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F4" s="26"/>
       <c r="G4" s="29"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="36"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="34"/>
       <c r="M4" s="39"/>
       <c r="N4" s="39"/>
-      <c r="O4" s="38"/>
+      <c r="O4" s="39"/>
       <c r="P4" s="37"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="2"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Q4" s="3"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="4"/>
+    </row>
+    <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>67</v>
       </c>
@@ -1724,52 +1905,26 @@
         <v>92</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F5" s="26"/>
-      <c r="G5" s="29" t="s">
-        <v>155</v>
-      </c>
-      <c r="H5" s="30">
-        <v>1</v>
-      </c>
-      <c r="I5" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="K5" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="L5" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="M5" s="39" t="s">
-        <v>36</v>
-      </c>
+      <c r="G5" s="29"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="39"/>
       <c r="N5" s="39"/>
       <c r="O5" s="38"/>
-      <c r="P5" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>6</v>
-      </c>
-      <c r="R5" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="S5" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="T5" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="U5" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="P5" s="37"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="2"/>
+    </row>
+    <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>67</v>
       </c>
@@ -1783,52 +1938,26 @@
         <v>92</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F6" s="26"/>
-      <c r="G6" s="29" t="s">
-        <v>132</v>
-      </c>
-      <c r="H6" s="30">
-        <v>2</v>
-      </c>
-      <c r="I6" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="31" t="s">
-        <v>161</v>
-      </c>
-      <c r="K6" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="L6" s="36" t="s">
-        <v>32</v>
-      </c>
+      <c r="G6" s="29"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="36"/>
       <c r="M6" s="39"/>
-      <c r="N6" s="39" t="s">
-        <v>62</v>
-      </c>
+      <c r="N6" s="39"/>
       <c r="O6" s="38"/>
-      <c r="P6" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>6</v>
-      </c>
-      <c r="R6" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="S6" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="T6" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P6" s="37"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="2"/>
+    </row>
+    <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>67</v>
       </c>
@@ -1839,62 +1968,110 @@
         <v>91</v>
       </c>
       <c r="D7" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="F7" s="26"/>
+      <c r="G7" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="H7" s="30">
+        <v>2</v>
+      </c>
+      <c r="I7" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="K7" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="L7" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="M7" s="39"/>
+      <c r="N7" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="O7" s="38"/>
+      <c r="P7" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>6</v>
+      </c>
+      <c r="R7" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="S7" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="T7" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" s="88" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="72" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="73" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="74" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="74" t="s">
         <v>93</v>
       </c>
-      <c r="E7" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="39"/>
-      <c r="N7" s="39"/>
-      <c r="O7" s="38"/>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="2"/>
-    </row>
-    <row r="8" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="38"/>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="2"/>
-    </row>
-    <row r="9" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="75"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="77" t="s">
+        <v>214</v>
+      </c>
+      <c r="H8" s="78">
+        <v>3</v>
+      </c>
+      <c r="I8" s="78" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="79" t="s">
+        <v>215</v>
+      </c>
+      <c r="K8" s="80" t="s">
+        <v>69</v>
+      </c>
+      <c r="L8" s="81"/>
+      <c r="M8" s="82"/>
+      <c r="N8" s="82"/>
+      <c r="O8" s="83" t="s">
+        <v>216</v>
+      </c>
+      <c r="P8" s="84" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q8" s="85">
+        <v>6</v>
+      </c>
+      <c r="R8" s="86" t="s">
+        <v>152</v>
+      </c>
+      <c r="S8" s="86" t="s">
+        <v>217</v>
+      </c>
+      <c r="T8" s="86" t="s">
+        <v>218</v>
+      </c>
+      <c r="U8" s="87" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>67</v>
       </c>
@@ -1908,50 +2085,26 @@
         <v>93</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F9" s="26"/>
-      <c r="G9" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="H9" s="30">
-        <v>3</v>
-      </c>
-      <c r="I9" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="J9" s="31" t="s">
-        <v>163</v>
-      </c>
-      <c r="K9" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="L9" s="36" t="s">
-        <v>32</v>
-      </c>
+      <c r="G9" s="29"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="36"/>
       <c r="M9" s="39"/>
-      <c r="N9" s="39" t="s">
-        <v>62</v>
-      </c>
+      <c r="N9" s="39"/>
       <c r="O9" s="38"/>
       <c r="P9" s="37"/>
-      <c r="Q9" s="1">
-        <v>6</v>
-      </c>
-      <c r="R9" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="S9" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="T9" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="U9" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q9" s="1"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="2"/>
+    </row>
+    <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>67</v>
       </c>
@@ -1962,10 +2115,10 @@
         <v>91</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F10" s="26"/>
       <c r="G10" s="29"/>
@@ -1984,7 +2137,7 @@
       <c r="T10" s="13"/>
       <c r="U10" s="2"/>
     </row>
-    <row r="11" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>67</v>
       </c>
@@ -1995,88 +2148,96 @@
         <v>91</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F11" s="26"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="39"/>
+      <c r="G11" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="H11" s="30">
+        <v>4</v>
+      </c>
+      <c r="I11" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="K11" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="L11" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="M11" s="39" t="s">
+        <v>36</v>
+      </c>
       <c r="N11" s="39"/>
       <c r="O11" s="38"/>
       <c r="P11" s="37"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="13"/>
-      <c r="T11" s="13"/>
-      <c r="U11" s="2"/>
-    </row>
-    <row r="12" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="Q11" s="1">
+        <v>6</v>
+      </c>
+      <c r="R11" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="S11" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="T11" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" s="88" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="72" t="s">
         <v>67</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="73" t="s">
         <v>90</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="74" t="s">
         <v>91</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="74" t="s">
         <v>94</v>
       </c>
-      <c r="E12" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="F12" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="G12" s="29" t="s">
-        <v>134</v>
-      </c>
-      <c r="H12" s="30">
-        <v>4</v>
-      </c>
-      <c r="I12" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="J12" s="31" t="s">
-        <v>166</v>
-      </c>
-      <c r="K12" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="L12" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="38"/>
-      <c r="P12" s="37" t="s">
+      <c r="E12" s="75"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="77" t="s">
+        <v>220</v>
+      </c>
+      <c r="H12" s="78">
+        <v>5</v>
+      </c>
+      <c r="I12" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="R12" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="S12" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="T12" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J12" s="79" t="s">
+        <v>221</v>
+      </c>
+      <c r="K12" s="80" t="s">
+        <v>69</v>
+      </c>
+      <c r="L12" s="81" t="s">
+        <v>31</v>
+      </c>
+      <c r="M12" s="82"/>
+      <c r="N12" s="82"/>
+      <c r="O12" s="83"/>
+      <c r="P12" s="84"/>
+      <c r="Q12" s="85"/>
+      <c r="R12" s="86"/>
+      <c r="S12" s="86"/>
+      <c r="T12" s="86"/>
+      <c r="U12" s="87"/>
+    </row>
+    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>67</v>
       </c>
@@ -2090,54 +2251,26 @@
         <v>94</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="F13" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="G13" s="29" t="s">
-        <v>167</v>
-      </c>
-      <c r="H13" s="30">
-        <v>5</v>
-      </c>
-      <c r="I13" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="J13" s="40" t="s">
-        <v>168</v>
-      </c>
-      <c r="K13" s="42" t="s">
-        <v>69</v>
-      </c>
-      <c r="L13" s="43" t="s">
-        <v>32</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="F13" s="26"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="36"/>
       <c r="M13" s="39"/>
-      <c r="N13" s="41" t="s">
-        <v>73</v>
-      </c>
+      <c r="N13" s="39"/>
       <c r="O13" s="38"/>
-      <c r="P13" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q13" s="1">
-        <v>6</v>
-      </c>
-      <c r="R13" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="S13" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="T13" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="U13" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="P13" s="37"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="13"/>
+      <c r="U13" s="2"/>
+    </row>
+    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>67</v>
       </c>
@@ -2151,54 +2284,26 @@
         <v>94</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="F14" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="G14" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="H14" s="30">
-        <v>6</v>
-      </c>
-      <c r="I14" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="J14" s="31" t="s">
-        <v>170</v>
-      </c>
-      <c r="K14" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="L14" s="36" t="s">
-        <v>31</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="F14" s="26"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="36"/>
       <c r="M14" s="39"/>
       <c r="N14" s="39"/>
       <c r="O14" s="38"/>
-      <c r="P14" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="R14" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="S14" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="T14" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="U14" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="V14" s="5"/>
-      <c r="W14" s="5"/>
-    </row>
-    <row r="15" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="P14" s="37"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="2"/>
+    </row>
+    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>67</v>
       </c>
@@ -2215,25 +2320,25 @@
         <v>109</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="H15" s="30">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I15" s="30" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J15" s="31" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="K15" s="35" t="s">
         <v>70</v>
       </c>
       <c r="L15" s="36" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M15" s="39"/>
       <c r="N15" s="39"/>
@@ -2242,23 +2347,22 @@
         <v>19</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="R15" s="13" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="S15" s="13" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="T15" s="13" t="s">
-        <v>202</v>
+        <v>134</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="V15" s="5"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
         <v>67</v>
       </c>
@@ -2275,50 +2379,51 @@
         <v>109</v>
       </c>
       <c r="F16" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G16" s="29" t="s">
-        <v>136</v>
+        <v>166</v>
       </c>
       <c r="H16" s="30">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I16" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="31" t="s">
-        <v>169</v>
-      </c>
-      <c r="K16" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="L16" s="36" t="s">
+      <c r="J16" s="40" t="s">
+        <v>167</v>
+      </c>
+      <c r="K16" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="L16" s="43" t="s">
         <v>32</v>
       </c>
       <c r="M16" s="39"/>
-      <c r="N16" s="39"/>
+      <c r="N16" s="41" t="s">
+        <v>73</v>
+      </c>
       <c r="O16" s="38"/>
       <c r="P16" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q16" s="1" t="s">
-        <v>199</v>
+        <v>20</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>6</v>
       </c>
       <c r="R16" s="13" t="s">
-        <v>200</v>
+        <v>152</v>
       </c>
       <c r="S16" s="13" t="s">
-        <v>201</v>
+        <v>153</v>
       </c>
       <c r="T16" s="13" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="V16" s="5"/>
-    </row>
-    <row r="17" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>67</v>
       </c>
@@ -2332,26 +2437,54 @@
         <v>94</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="36"/>
+        <v>109</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="G17" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="H17" s="30">
+        <v>8</v>
+      </c>
+      <c r="I17" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="K17" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L17" s="36" t="s">
+        <v>31</v>
+      </c>
       <c r="M17" s="39"/>
       <c r="N17" s="39"/>
       <c r="O17" s="38"/>
-      <c r="P17" s="37"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="13"/>
-      <c r="S17" s="13"/>
-      <c r="T17" s="13"/>
-      <c r="U17" s="2"/>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="P17" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="R17" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="S17" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="T17" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="U17" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+    </row>
+    <row r="18" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>67</v>
       </c>
@@ -2365,52 +2498,53 @@
         <v>94</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="F18" s="26"/>
+        <v>109</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>124</v>
+      </c>
       <c r="G18" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H18" s="30">
         <v>9</v>
       </c>
       <c r="I18" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J18" s="31" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K18" s="35" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L18" s="36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M18" s="39"/>
-      <c r="N18" s="39" t="s">
-        <v>62</v>
-      </c>
+      <c r="N18" s="39"/>
       <c r="O18" s="38"/>
       <c r="P18" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="Q18" s="1">
-        <v>6</v>
+      <c r="Q18" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="R18" s="13" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
       <c r="S18" s="13" t="s">
-        <v>153</v>
+        <v>198</v>
       </c>
       <c r="T18" s="13" t="s">
-        <v>173</v>
+        <v>199</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+      <c r="V18" s="5"/>
+    </row>
+    <row r="19" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>67</v>
       </c>
@@ -2421,14 +2555,16 @@
         <v>91</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="F19" s="26"/>
+        <v>109</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>124</v>
+      </c>
       <c r="G19" s="29" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H19" s="30">
         <v>10</v>
@@ -2437,7 +2573,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="31" t="s">
-        <v>140</v>
+        <v>168</v>
       </c>
       <c r="K19" s="35" t="s">
         <v>70</v>
@@ -2452,23 +2588,23 @@
         <v>19</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="R19" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="S19" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="T19" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="S19" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="T19" s="13" t="s">
-        <v>140</v>
-      </c>
       <c r="U19" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="V19" s="5"/>
     </row>
-    <row r="20" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>67</v>
       </c>
@@ -2479,10 +2615,10 @@
         <v>91</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F20" s="26"/>
       <c r="G20" s="29"/>
@@ -2501,7 +2637,7 @@
       <c r="T20" s="13"/>
       <c r="U20" s="2"/>
     </row>
-    <row r="21" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>67</v>
       </c>
@@ -2512,62 +2648,112 @@
         <v>91</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F21" s="26"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="36"/>
+      <c r="G21" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="H21" s="30">
+        <v>11</v>
+      </c>
+      <c r="I21" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="K21" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="L21" s="36" t="s">
+        <v>32</v>
+      </c>
       <c r="M21" s="39"/>
-      <c r="N21" s="39"/>
+      <c r="N21" s="39" t="s">
+        <v>62</v>
+      </c>
       <c r="O21" s="38"/>
-      <c r="P21" s="37"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="13"/>
-      <c r="T21" s="13"/>
-      <c r="U21" s="2"/>
-    </row>
-    <row r="22" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
+      <c r="P21" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>6</v>
+      </c>
+      <c r="R21" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="S21" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="T21" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="U21" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" s="88" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="72" t="s">
         <v>67</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="73" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="74" t="s">
         <v>91</v>
       </c>
-      <c r="D22" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="E22" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="F22" s="26"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="35"/>
-      <c r="L22" s="36"/>
-      <c r="M22" s="39"/>
-      <c r="N22" s="39"/>
-      <c r="O22" s="38"/>
-      <c r="P22" s="37"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="13"/>
-      <c r="S22" s="13"/>
-      <c r="T22" s="13"/>
-      <c r="U22" s="2"/>
-    </row>
-    <row r="23" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+      <c r="D22" s="74" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" s="75"/>
+      <c r="F22" s="76"/>
+      <c r="G22" s="77" t="s">
+        <v>223</v>
+      </c>
+      <c r="H22" s="78">
+        <v>12</v>
+      </c>
+      <c r="I22" s="78" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" s="79" t="s">
+        <v>224</v>
+      </c>
+      <c r="K22" s="80" t="s">
+        <v>69</v>
+      </c>
+      <c r="L22" s="81" t="s">
+        <v>31</v>
+      </c>
+      <c r="M22" s="82" t="s">
+        <v>46</v>
+      </c>
+      <c r="N22" s="82"/>
+      <c r="O22" s="83"/>
+      <c r="P22" s="84" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q22" s="88">
+        <v>6</v>
+      </c>
+      <c r="R22" s="88" t="s">
+        <v>157</v>
+      </c>
+      <c r="S22" s="88" t="s">
+        <v>158</v>
+      </c>
+      <c r="T22" s="89" t="s">
+        <v>225</v>
+      </c>
+      <c r="U22" s="88" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>67</v>
       </c>
@@ -2578,54 +2764,56 @@
         <v>91</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="F23" s="26"/>
       <c r="G23" s="29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H23" s="30">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I23" s="30" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J23" s="31" t="s">
-        <v>174</v>
+        <v>140</v>
       </c>
       <c r="K23" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="L23" s="36"/>
-      <c r="M23" s="39"/>
+      <c r="L23" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="M23" s="39" t="s">
+        <v>62</v>
+      </c>
       <c r="N23" s="39"/>
-      <c r="O23" s="38" t="s">
-        <v>207</v>
-      </c>
+      <c r="O23" s="38"/>
       <c r="P23" s="37" t="s">
         <v>19</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="R23" s="13" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="S23" s="13" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="T23" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U23" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="V23" s="5"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>67</v>
       </c>
@@ -2639,51 +2827,26 @@
         <v>96</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F24" s="26"/>
-      <c r="G24" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="H24" s="30">
-        <v>12</v>
-      </c>
-      <c r="I24" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="J24" s="31" t="s">
-        <v>175</v>
-      </c>
-      <c r="K24" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="L24" s="36" t="s">
-        <v>31</v>
-      </c>
+      <c r="G24" s="29"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="36"/>
       <c r="M24" s="39"/>
       <c r="N24" s="39"/>
       <c r="O24" s="38"/>
-      <c r="P24" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q24" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="R24" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="S24" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="T24" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="U24" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="V24" s="5"/>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="P24" s="37"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="13"/>
+      <c r="S24" s="13"/>
+      <c r="T24" s="13"/>
+      <c r="U24" s="2"/>
+    </row>
+    <row r="25" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>67</v>
       </c>
@@ -2697,52 +2860,26 @@
         <v>96</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F25" s="26"/>
-      <c r="G25" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="H25" s="30">
-        <v>13</v>
-      </c>
-      <c r="I25" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="J25" s="31" t="s">
-        <v>176</v>
-      </c>
-      <c r="K25" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="L25" s="36" t="s">
-        <v>32</v>
-      </c>
+      <c r="G25" s="29"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="36"/>
       <c r="M25" s="39"/>
       <c r="N25" s="39"/>
       <c r="O25" s="38"/>
-      <c r="P25" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q25" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="R25" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="S25" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="T25" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="U25" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="V25" s="5"/>
-      <c r="W25" s="5"/>
-    </row>
-    <row r="26" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P25" s="37"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="13"/>
+      <c r="S25" s="13"/>
+      <c r="T25" s="13"/>
+      <c r="U25" s="2"/>
+    </row>
+    <row r="26" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
         <v>67</v>
       </c>
@@ -2756,11 +2893,9 @@
         <v>96</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="F26" s="26" t="s">
-        <v>125</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="F26" s="26"/>
       <c r="G26" s="29"/>
       <c r="H26" s="30"/>
       <c r="I26" s="30"/>
@@ -2777,7 +2912,7 @@
       <c r="T26" s="13"/>
       <c r="U26" s="2"/>
     </row>
-    <row r="27" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
         <v>67</v>
       </c>
@@ -2791,28 +2926,51 @@
         <v>96</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="F27" s="26" t="s">
-        <v>126</v>
-      </c>
-      <c r="G27" s="29"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="30"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="35"/>
+        <v>114</v>
+      </c>
+      <c r="F27" s="26"/>
+      <c r="G27" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="H27" s="30">
+        <v>14</v>
+      </c>
+      <c r="I27" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="J27" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="K27" s="35" t="s">
+        <v>70</v>
+      </c>
       <c r="L27" s="36"/>
       <c r="M27" s="39"/>
       <c r="N27" s="39"/>
-      <c r="O27" s="38"/>
-      <c r="P27" s="37"/>
-      <c r="Q27" s="1"/>
-      <c r="R27" s="13"/>
-      <c r="S27" s="13"/>
-      <c r="T27" s="13"/>
-      <c r="U27" s="2"/>
-    </row>
-    <row r="28" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O27" s="38" t="s">
+        <v>204</v>
+      </c>
+      <c r="P27" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="R27" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="S27" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="T27" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="U27" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="V27" s="5"/>
+    </row>
+    <row r="28" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>67</v>
       </c>
@@ -2826,28 +2984,51 @@
         <v>96</v>
       </c>
       <c r="E28" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="F28" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="G28" s="29"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="30"/>
-      <c r="J28" s="31"/>
-      <c r="K28" s="35"/>
-      <c r="L28" s="36"/>
+        <v>115</v>
+      </c>
+      <c r="F28" s="26"/>
+      <c r="G28" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="H28" s="30">
+        <v>15</v>
+      </c>
+      <c r="I28" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="J28" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="K28" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L28" s="36" t="s">
+        <v>31</v>
+      </c>
       <c r="M28" s="39"/>
       <c r="N28" s="39"/>
       <c r="O28" s="38"/>
-      <c r="P28" s="37"/>
-      <c r="Q28" s="1"/>
-      <c r="R28" s="13"/>
-      <c r="S28" s="13"/>
-      <c r="T28" s="13"/>
-      <c r="U28" s="2"/>
-    </row>
-    <row r="29" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P28" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="R28" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="S28" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="T28" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="U28" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="V28" s="5"/>
+    </row>
+    <row r="29" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>67</v>
       </c>
@@ -2861,28 +3042,52 @@
         <v>96</v>
       </c>
       <c r="E29" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="F29" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="G29" s="29"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="31"/>
-      <c r="K29" s="35"/>
-      <c r="L29" s="36"/>
+        <v>115</v>
+      </c>
+      <c r="F29" s="26"/>
+      <c r="G29" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="H29" s="30">
+        <v>16</v>
+      </c>
+      <c r="I29" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J29" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="K29" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L29" s="36" t="s">
+        <v>32</v>
+      </c>
       <c r="M29" s="39"/>
       <c r="N29" s="39"/>
       <c r="O29" s="38"/>
-      <c r="P29" s="37"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="13"/>
-      <c r="S29" s="13"/>
-      <c r="T29" s="13"/>
-      <c r="U29" s="2"/>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="P29" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="R29" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="S29" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="T29" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="U29" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="V29" s="5"/>
+      <c r="W29" s="5"/>
+    </row>
+    <row r="30" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>67</v>
       </c>
@@ -2896,52 +3101,28 @@
         <v>96</v>
       </c>
       <c r="E30" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="F30" s="26"/>
-      <c r="G30" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="H30" s="30">
-        <v>14</v>
-      </c>
-      <c r="I30" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="J30" s="31" t="s">
-        <v>177</v>
-      </c>
-      <c r="K30" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="L30" s="36" t="s">
-        <v>32</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="F30" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="G30" s="29"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="31"/>
+      <c r="K30" s="35"/>
+      <c r="L30" s="36"/>
       <c r="M30" s="39"/>
-      <c r="N30" s="39" t="s">
-        <v>62</v>
-      </c>
+      <c r="N30" s="39"/>
       <c r="O30" s="38"/>
-      <c r="P30" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q30" s="1">
-        <v>6</v>
-      </c>
-      <c r="R30" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="S30" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="T30" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="U30" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="P30" s="37"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="13"/>
+      <c r="S30" s="13"/>
+      <c r="T30" s="13"/>
+      <c r="U30" s="2"/>
+    </row>
+    <row r="31" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
         <v>67</v>
       </c>
@@ -2952,52 +3133,31 @@
         <v>91</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="E31" s="25"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="H31" s="30">
-        <v>15</v>
-      </c>
-      <c r="I31" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="J31" s="31" t="s">
-        <v>179</v>
-      </c>
-      <c r="K31" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="L31" s="36" t="s">
-        <v>32</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="F31" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="G31" s="29"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="31"/>
+      <c r="K31" s="35"/>
+      <c r="L31" s="36"/>
       <c r="M31" s="39"/>
       <c r="N31" s="39"/>
       <c r="O31" s="38"/>
-      <c r="P31" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q31" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="R31" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="S31" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="T31" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="U31" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="V31" s="5"/>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="P31" s="37"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="13"/>
+      <c r="S31" s="13"/>
+      <c r="T31" s="13"/>
+      <c r="U31" s="2"/>
+    </row>
+    <row r="32" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
         <v>67</v>
       </c>
@@ -3008,52 +3168,31 @@
         <v>91</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="E32" s="25"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="29" t="s">
-        <v>145</v>
-      </c>
-      <c r="H32" s="30">
-        <v>16</v>
-      </c>
-      <c r="I32" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="J32" s="31" t="s">
-        <v>180</v>
-      </c>
-      <c r="K32" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="L32" s="36" t="s">
-        <v>32</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="E32" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="F32" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="G32" s="29"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="35"/>
+      <c r="L32" s="36"/>
       <c r="M32" s="39"/>
       <c r="N32" s="39"/>
       <c r="O32" s="38"/>
-      <c r="P32" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q32" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="R32" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="S32" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="T32" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="U32" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="V32" s="5"/>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="P32" s="37"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="13"/>
+      <c r="S32" s="13"/>
+      <c r="T32" s="13"/>
+      <c r="U32" s="2"/>
+    </row>
+    <row r="33" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
         <v>67</v>
       </c>
@@ -3064,54 +3203,31 @@
         <v>91</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E33" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="F33" s="26"/>
-      <c r="G33" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="H33" s="30">
-        <v>17</v>
-      </c>
-      <c r="I33" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="J33" s="31" t="s">
-        <v>181</v>
-      </c>
-      <c r="K33" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="L33" s="36" t="s">
-        <v>32</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="F33" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="G33" s="29"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="31"/>
+      <c r="K33" s="35"/>
+      <c r="L33" s="36"/>
       <c r="M33" s="39"/>
       <c r="N33" s="39"/>
       <c r="O33" s="38"/>
-      <c r="P33" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q33" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="R33" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="S33" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="T33" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="U33" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="V33" s="5"/>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="P33" s="37"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="13"/>
+      <c r="S33" s="13"/>
+      <c r="T33" s="13"/>
+      <c r="U33" s="2"/>
+    </row>
+    <row r="34" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
         <v>67</v>
       </c>
@@ -3122,88 +3238,112 @@
         <v>91</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E34" s="25" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="F34" s="26"/>
       <c r="G34" s="29" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H34" s="30">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I34" s="30" t="s">
         <v>20</v>
       </c>
       <c r="J34" s="31" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="K34" s="35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L34" s="36" t="s">
         <v>32</v>
       </c>
       <c r="M34" s="39"/>
-      <c r="N34" s="39"/>
+      <c r="N34" s="39" t="s">
+        <v>62</v>
+      </c>
       <c r="O34" s="38"/>
       <c r="P34" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="Q34" s="1" t="s">
-        <v>199</v>
+      <c r="Q34" s="1">
+        <v>6</v>
       </c>
       <c r="R34" s="13" t="s">
-        <v>200</v>
+        <v>152</v>
       </c>
       <c r="S34" s="13" t="s">
-        <v>201</v>
+        <v>153</v>
       </c>
       <c r="T34" s="13" t="s">
-        <v>206</v>
+        <v>177</v>
       </c>
       <c r="U34" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="V34" s="5"/>
-    </row>
-    <row r="35" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="18" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" s="88" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="72" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="73" t="s">
         <v>90</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="74" t="s">
         <v>91</v>
       </c>
-      <c r="D35" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="E35" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="F35" s="26"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="30"/>
-      <c r="J35" s="28"/>
-      <c r="K35" s="35"/>
-      <c r="L35" s="36"/>
-      <c r="M35" s="39"/>
-      <c r="N35" s="39"/>
-      <c r="O35" s="38"/>
-      <c r="P35" s="37"/>
-      <c r="Q35" s="1"/>
-      <c r="R35" s="13"/>
-      <c r="S35" s="13"/>
-      <c r="T35" s="13"/>
-      <c r="U35" s="2"/>
-      <c r="V35" s="5"/>
-    </row>
-    <row r="36" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D35" s="74" t="s">
+        <v>97</v>
+      </c>
+      <c r="E35" s="75"/>
+      <c r="F35" s="76"/>
+      <c r="G35" s="77" t="s">
+        <v>230</v>
+      </c>
+      <c r="H35" s="78">
+        <v>18</v>
+      </c>
+      <c r="I35" s="78" t="s">
+        <v>19</v>
+      </c>
+      <c r="J35" s="79" t="s">
+        <v>231</v>
+      </c>
+      <c r="K35" s="80" t="s">
+        <v>69</v>
+      </c>
+      <c r="L35" s="81" t="s">
+        <v>31</v>
+      </c>
+      <c r="M35" s="82" t="s">
+        <v>36</v>
+      </c>
+      <c r="N35" s="82"/>
+      <c r="O35" s="83"/>
+      <c r="P35" s="84" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q35" s="85">
+        <v>6</v>
+      </c>
+      <c r="R35" s="86" t="s">
+        <v>157</v>
+      </c>
+      <c r="S35" s="86" t="s">
+        <v>158</v>
+      </c>
+      <c r="T35" s="86" t="s">
+        <v>222</v>
+      </c>
+      <c r="U35" s="87" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
         <v>67</v>
       </c>
@@ -3214,14 +3354,12 @@
         <v>91</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="E36" s="25" t="s">
-        <v>119</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="E36" s="25"/>
       <c r="F36" s="26"/>
-      <c r="G36" s="44" t="s">
-        <v>185</v>
+      <c r="G36" s="29" t="s">
+        <v>144</v>
       </c>
       <c r="H36" s="30">
         <v>19</v>
@@ -3230,40 +3368,38 @@
         <v>20</v>
       </c>
       <c r="J36" s="31" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="K36" s="35" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L36" s="36" t="s">
         <v>32</v>
       </c>
       <c r="M36" s="39"/>
-      <c r="N36" s="39" t="s">
-        <v>53</v>
-      </c>
+      <c r="N36" s="39"/>
       <c r="O36" s="38"/>
       <c r="P36" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q36" s="1">
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="Q36" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="R36" s="13" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
       <c r="S36" s="13" t="s">
-        <v>153</v>
+        <v>198</v>
       </c>
       <c r="T36" s="13" t="s">
-        <v>186</v>
+        <v>144</v>
       </c>
       <c r="U36" s="2" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="V36" s="5"/>
     </row>
-    <row r="37" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
         <v>67</v>
       </c>
@@ -3274,30 +3410,52 @@
         <v>91</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="E37" s="25" t="s">
-        <v>120</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="E37" s="25"/>
       <c r="F37" s="26"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="30"/>
-      <c r="I37" s="30"/>
-      <c r="J37" s="31"/>
-      <c r="K37" s="35"/>
-      <c r="L37" s="36"/>
+      <c r="G37" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="H37" s="30">
+        <v>20</v>
+      </c>
+      <c r="I37" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J37" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="K37" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L37" s="36" t="s">
+        <v>32</v>
+      </c>
       <c r="M37" s="39"/>
       <c r="N37" s="39"/>
       <c r="O37" s="38"/>
-      <c r="P37" s="37"/>
-      <c r="Q37" s="1"/>
-      <c r="R37" s="13"/>
-      <c r="S37" s="13"/>
-      <c r="T37" s="13"/>
-      <c r="U37" s="2"/>
+      <c r="P37" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="R37" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="S37" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="T37" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="U37" s="2" t="s">
+        <v>164</v>
+      </c>
       <c r="V37" s="5"/>
     </row>
-    <row r="38" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
         <v>67</v>
       </c>
@@ -3308,30 +3466,54 @@
         <v>91</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E38" s="25" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="F38" s="26"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="30"/>
-      <c r="J38" s="31"/>
-      <c r="K38" s="35"/>
-      <c r="L38" s="36"/>
+      <c r="G38" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="H38" s="30">
+        <v>21</v>
+      </c>
+      <c r="I38" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J38" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="K38" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L38" s="36" t="s">
+        <v>32</v>
+      </c>
       <c r="M38" s="39"/>
       <c r="N38" s="39"/>
       <c r="O38" s="38"/>
-      <c r="P38" s="37"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="13"/>
-      <c r="S38" s="13"/>
-      <c r="T38" s="13"/>
-      <c r="U38" s="2"/>
+      <c r="P38" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q38" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="R38" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="S38" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="T38" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="U38" s="2" t="s">
+        <v>164</v>
+      </c>
       <c r="V38" s="5"/>
     </row>
-    <row r="39" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
         <v>67</v>
       </c>
@@ -3345,11 +3527,9 @@
         <v>98</v>
       </c>
       <c r="E39" s="25" t="s">
-        <v>122</v>
-      </c>
-      <c r="F39" s="26" t="s">
-        <v>129</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="F39" s="26"/>
       <c r="G39" s="29"/>
       <c r="H39" s="30"/>
       <c r="I39" s="30"/>
@@ -3367,7 +3547,7 @@
       <c r="U39" s="2"/>
       <c r="V39" s="5"/>
     </row>
-    <row r="40" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
         <v>67</v>
       </c>
@@ -3380,14 +3560,14 @@
       <c r="D40" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="E40" s="25"/>
-      <c r="F40" s="26" t="s">
-        <v>130</v>
-      </c>
+      <c r="E40" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="F40" s="26"/>
       <c r="G40" s="29"/>
       <c r="H40" s="30"/>
       <c r="I40" s="30"/>
-      <c r="J40" s="31"/>
+      <c r="J40" s="28"/>
       <c r="K40" s="35"/>
       <c r="L40" s="36"/>
       <c r="M40" s="39"/>
@@ -3401,7 +3581,7 @@
       <c r="U40" s="2"/>
       <c r="V40" s="5"/>
     </row>
-    <row r="41" spans="1:22" s="5" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
         <v>67</v>
       </c>
@@ -3414,55 +3594,28 @@
       <c r="D41" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="E41" s="25"/>
-      <c r="F41" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="G41" s="29" t="s">
-        <v>183</v>
-      </c>
-      <c r="H41" s="30">
-        <v>20</v>
-      </c>
-      <c r="I41" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="J41" s="31" t="s">
-        <v>188</v>
-      </c>
-      <c r="K41" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="L41" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="M41" s="39" t="s">
-        <v>44</v>
-      </c>
+      <c r="E41" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="F41" s="26"/>
+      <c r="G41" s="44"/>
+      <c r="H41" s="30"/>
+      <c r="I41" s="30"/>
+      <c r="J41" s="31"/>
+      <c r="K41" s="35"/>
+      <c r="L41" s="36"/>
+      <c r="M41" s="39"/>
       <c r="N41" s="39"/>
-      <c r="O41" s="38" t="s">
-        <v>189</v>
-      </c>
-      <c r="P41" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q41" s="1">
-        <v>6</v>
-      </c>
-      <c r="R41" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="S41" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="T41" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="U41" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="O41" s="38"/>
+      <c r="P41" s="37"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="13"/>
+      <c r="S41" s="13"/>
+      <c r="T41" s="13"/>
+      <c r="U41" s="2"/>
+      <c r="V41" s="5"/>
+    </row>
+    <row r="42" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
         <v>67</v>
       </c>
@@ -3476,53 +3629,27 @@
         <v>98</v>
       </c>
       <c r="E42" s="25" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="F42" s="26"/>
-      <c r="G42" s="29" t="s">
-        <v>148</v>
-      </c>
-      <c r="H42" s="30">
-        <v>21</v>
-      </c>
-      <c r="I42" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="J42" s="31" t="s">
-        <v>191</v>
-      </c>
-      <c r="K42" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="L42" s="36" t="s">
-        <v>32</v>
-      </c>
+      <c r="G42" s="29"/>
+      <c r="H42" s="30"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="31"/>
+      <c r="K42" s="35"/>
+      <c r="L42" s="36"/>
       <c r="M42" s="39"/>
-      <c r="N42" s="39" t="s">
-        <v>62</v>
-      </c>
+      <c r="N42" s="39"/>
       <c r="O42" s="38"/>
-      <c r="P42" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q42" s="1">
-        <v>6</v>
-      </c>
-      <c r="R42" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="S42" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="T42" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="U42" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="P42" s="37"/>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="13"/>
+      <c r="S42" s="13"/>
+      <c r="T42" s="13"/>
+      <c r="U42" s="2"/>
       <c r="V42" s="5"/>
     </row>
-    <row r="43" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
         <v>67</v>
       </c>
@@ -3532,53 +3659,31 @@
       <c r="C43" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="D43" s="45" t="s">
-        <v>208</v>
-      </c>
-      <c r="E43" s="25"/>
+      <c r="D43" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="E43" s="25" t="s">
+        <v>121</v>
+      </c>
       <c r="F43" s="26"/>
-      <c r="G43" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="H43" s="30">
-        <v>22</v>
-      </c>
-      <c r="I43" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="J43" s="31" t="s">
-        <v>194</v>
-      </c>
-      <c r="K43" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="L43" s="36" t="s">
-        <v>32</v>
-      </c>
+      <c r="G43" s="29"/>
+      <c r="H43" s="30"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="31"/>
+      <c r="K43" s="35"/>
+      <c r="L43" s="36"/>
       <c r="M43" s="39"/>
       <c r="N43" s="39"/>
       <c r="O43" s="38"/>
-      <c r="P43" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q43" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="R43" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="S43" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="T43" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="U43" s="2" t="s">
-        <v>165</v>
-      </c>
+      <c r="P43" s="37"/>
+      <c r="Q43" s="1"/>
+      <c r="R43" s="13"/>
+      <c r="S43" s="13"/>
+      <c r="T43" s="13"/>
+      <c r="U43" s="2"/>
       <c r="V43" s="5"/>
     </row>
-    <row r="44" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
         <v>67</v>
       </c>
@@ -3588,53 +3693,33 @@
       <c r="C44" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="D44" s="45" t="s">
-        <v>208</v>
-      </c>
-      <c r="E44" s="25"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="29" t="s">
-        <v>149</v>
-      </c>
-      <c r="H44" s="30">
-        <v>23</v>
-      </c>
-      <c r="I44" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="J44" s="31" t="s">
-        <v>195</v>
-      </c>
-      <c r="K44" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="L44" s="36" t="s">
-        <v>32</v>
-      </c>
+      <c r="D44" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="E44" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="F44" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="G44" s="29"/>
+      <c r="H44" s="30"/>
+      <c r="I44" s="30"/>
+      <c r="J44" s="31"/>
+      <c r="K44" s="35"/>
+      <c r="L44" s="36"/>
       <c r="M44" s="39"/>
       <c r="N44" s="39"/>
       <c r="O44" s="38"/>
-      <c r="P44" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q44" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="R44" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="S44" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="T44" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="U44" s="2" t="s">
-        <v>165</v>
-      </c>
+      <c r="P44" s="37"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="13"/>
+      <c r="S44" s="13"/>
+      <c r="T44" s="13"/>
+      <c r="U44" s="2"/>
       <c r="V44" s="5"/>
     </row>
-    <row r="45" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
         <v>67</v>
       </c>
@@ -3644,55 +3729,31 @@
       <c r="C45" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="D45" s="45" t="s">
-        <v>208</v>
+      <c r="D45" s="20" t="s">
+        <v>98</v>
       </c>
       <c r="E45" s="25"/>
-      <c r="F45" s="26"/>
-      <c r="G45" s="29" t="s">
-        <v>213</v>
-      </c>
-      <c r="H45" s="30">
-        <v>24</v>
-      </c>
-      <c r="I45" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="J45" s="31" t="s">
-        <v>214</v>
-      </c>
-      <c r="K45" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="L45" s="36" t="s">
-        <v>32</v>
-      </c>
+      <c r="F45" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="G45" s="29"/>
+      <c r="H45" s="30"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="31"/>
+      <c r="K45" s="35"/>
+      <c r="L45" s="36"/>
       <c r="M45" s="39"/>
-      <c r="N45" s="39" t="s">
-        <v>64</v>
-      </c>
+      <c r="N45" s="39"/>
       <c r="O45" s="38"/>
-      <c r="P45" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q45" s="1">
-        <v>6</v>
-      </c>
-      <c r="R45" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="S45" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="T45" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="U45" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="P45" s="37"/>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="13"/>
+      <c r="S45" s="13"/>
+      <c r="T45" s="13"/>
+      <c r="U45" s="2"/>
       <c r="V45" s="5"/>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
         <v>67</v>
       </c>
@@ -3702,373 +3763,622 @@
       <c r="C46" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="D46" s="45" t="s">
-        <v>208</v>
+      <c r="D46" s="20" t="s">
+        <v>98</v>
       </c>
       <c r="E46" s="25"/>
-      <c r="F46" s="26"/>
+      <c r="F46" s="26" t="s">
+        <v>131</v>
+      </c>
       <c r="G46" s="29" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="H46" s="30">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I46" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J46" s="31" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="K46" s="35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L46" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="M46" s="39"/>
+        <v>31</v>
+      </c>
+      <c r="M46" s="39" t="s">
+        <v>44</v>
+      </c>
       <c r="N46" s="39"/>
-      <c r="O46" s="38"/>
+      <c r="O46" s="38" t="s">
+        <v>188</v>
+      </c>
       <c r="P46" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="Q46" s="1" t="s">
-        <v>199</v>
+      <c r="Q46" s="1">
+        <v>6</v>
       </c>
       <c r="R46" s="13" t="s">
-        <v>200</v>
+        <v>157</v>
       </c>
       <c r="S46" s="13" t="s">
-        <v>201</v>
+        <v>158</v>
       </c>
       <c r="T46" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="U46" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" s="71" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="B47" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" s="57" t="s">
+        <v>91</v>
+      </c>
+      <c r="D47" s="57" t="s">
+        <v>98</v>
+      </c>
+      <c r="E47" s="58"/>
+      <c r="F47" s="59" t="s">
+        <v>131</v>
+      </c>
+      <c r="G47" s="60" t="s">
+        <v>147</v>
+      </c>
+      <c r="H47" s="61">
+        <v>23</v>
+      </c>
+      <c r="I47" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="J47" s="62" t="s">
+        <v>181</v>
+      </c>
+      <c r="K47" s="63" t="s">
+        <v>70</v>
+      </c>
+      <c r="L47" s="64" t="s">
+        <v>32</v>
+      </c>
+      <c r="M47" s="65"/>
+      <c r="N47" s="65"/>
+      <c r="O47" s="66"/>
+      <c r="P47" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q47" s="68" t="s">
+        <v>196</v>
+      </c>
+      <c r="R47" s="69" t="s">
+        <v>197</v>
+      </c>
+      <c r="S47" s="69" t="s">
+        <v>198</v>
+      </c>
+      <c r="T47" s="69" t="s">
+        <v>203</v>
+      </c>
+      <c r="U47" s="70" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" s="71" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="B48" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" s="57" t="s">
+        <v>91</v>
+      </c>
+      <c r="D48" s="57" t="s">
+        <v>98</v>
+      </c>
+      <c r="E48" s="58"/>
+      <c r="F48" s="59" t="s">
+        <v>131</v>
+      </c>
+      <c r="G48" s="91" t="s">
+        <v>184</v>
+      </c>
+      <c r="H48" s="61">
+        <v>24</v>
+      </c>
+      <c r="I48" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="J48" s="62" t="s">
+        <v>186</v>
+      </c>
+      <c r="K48" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="L48" s="64" t="s">
+        <v>32</v>
+      </c>
+      <c r="M48" s="65"/>
+      <c r="N48" s="65" t="s">
+        <v>53</v>
+      </c>
+      <c r="O48" s="66"/>
+      <c r="P48" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q48" s="68">
+        <v>6</v>
+      </c>
+      <c r="R48" s="69" t="s">
+        <v>152</v>
+      </c>
+      <c r="S48" s="69" t="s">
+        <v>153</v>
+      </c>
+      <c r="T48" s="69" t="s">
+        <v>185</v>
+      </c>
+      <c r="U48" s="70" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="B49" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="C49" s="57" t="s">
+        <v>91</v>
+      </c>
+      <c r="D49" s="57" t="s">
+        <v>98</v>
+      </c>
+      <c r="E49" s="58"/>
+      <c r="F49" s="59"/>
+      <c r="G49" s="60" t="s">
         <v>135</v>
       </c>
-      <c r="U46" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="V46" s="5"/>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A47" s="18" t="s">
+      <c r="H49" s="61">
+        <v>25</v>
+      </c>
+      <c r="I49" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="J49" s="62" t="s">
+        <v>193</v>
+      </c>
+      <c r="K49" s="63" t="s">
+        <v>70</v>
+      </c>
+      <c r="L49" s="64" t="s">
+        <v>32</v>
+      </c>
+      <c r="M49" s="65"/>
+      <c r="N49" s="65"/>
+      <c r="O49" s="66"/>
+      <c r="P49" s="90" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q49" s="68" t="s">
+        <v>196</v>
+      </c>
+      <c r="R49" s="69" t="s">
+        <v>197</v>
+      </c>
+      <c r="S49" s="69" t="s">
+        <v>198</v>
+      </c>
+      <c r="T49" s="69" t="s">
+        <v>135</v>
+      </c>
+      <c r="U49" s="70" t="s">
+        <v>164</v>
+      </c>
+      <c r="V49" s="5"/>
+    </row>
+    <row r="50" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B47" s="19" t="s">
+      <c r="B50" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C47" s="20" t="s">
+      <c r="C50" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="D47" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="E47" s="25"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="H47" s="30">
+      <c r="D50" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="E50" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="F50" s="26"/>
+      <c r="G50" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="H50" s="30">
         <v>26</v>
       </c>
-      <c r="I47" s="30" t="s">
+      <c r="I50" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="J47" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="K47" s="35" t="s">
+      <c r="J50" s="31" t="s">
+        <v>190</v>
+      </c>
+      <c r="K50" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="L47" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="M47" s="39"/>
-      <c r="N47" s="39"/>
-      <c r="O47" s="38"/>
-      <c r="P47" s="37" t="s">
+      <c r="L50" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="M50" s="39"/>
+      <c r="N50" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="O50" s="38"/>
+      <c r="P50" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="Q47" s="1"/>
-      <c r="R47" s="13"/>
-      <c r="S47" s="13"/>
-      <c r="T47" s="13"/>
-      <c r="U47" s="2"/>
-      <c r="V47" s="5"/>
-    </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A48" s="18" t="s">
+      <c r="Q50" s="1">
+        <v>6</v>
+      </c>
+      <c r="R50" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="S50" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="T50" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="U50" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="V50" s="5"/>
+    </row>
+    <row r="51" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B48" s="19" t="s">
+      <c r="B51" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C48" s="20" t="s">
+      <c r="C51" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="D48" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="E48" s="25"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="H48" s="30">
-        <v>27</v>
-      </c>
-      <c r="I48" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="J48" s="31" t="s">
-        <v>209</v>
-      </c>
-      <c r="K48" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="L48" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="M48" s="39"/>
-      <c r="N48" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="O48" s="38"/>
-      <c r="P48" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q48" s="1">
-        <v>6</v>
-      </c>
-      <c r="R48" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="S48" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="T48" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="U48" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="V48" s="5"/>
-    </row>
-    <row r="49" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B49" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="C49" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="D49" s="24"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="29" t="s">
-        <v>210</v>
-      </c>
-      <c r="H49" s="30">
-        <v>28</v>
-      </c>
-      <c r="I49" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="J49" s="31" t="s">
-        <v>211</v>
-      </c>
-      <c r="K49" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="L49" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="M49" s="39"/>
-      <c r="N49" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="O49" s="38"/>
-      <c r="P49" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q49" s="1">
-        <v>6</v>
-      </c>
-      <c r="R49" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="S49" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="T49" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="U49" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="21"/>
-      <c r="B50" s="22"/>
-      <c r="C50" s="23"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="25"/>
-      <c r="F50" s="26"/>
-      <c r="G50" s="29"/>
-      <c r="H50" s="30"/>
-      <c r="I50" s="30"/>
-      <c r="J50" s="31"/>
-      <c r="K50" s="35"/>
-      <c r="L50" s="36"/>
-      <c r="M50" s="39"/>
-      <c r="N50" s="39"/>
-      <c r="O50" s="38"/>
-      <c r="P50" s="37"/>
-      <c r="Q50" s="1"/>
-      <c r="R50" s="13"/>
-      <c r="S50" s="13"/>
-      <c r="T50" s="13"/>
-      <c r="U50" s="2"/>
-    </row>
-    <row r="51" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="21"/>
-      <c r="B51" s="22"/>
-      <c r="C51" s="23"/>
-      <c r="D51" s="24"/>
+      <c r="D51" s="45" t="s">
+        <v>205</v>
+      </c>
       <c r="E51" s="25"/>
       <c r="F51" s="26"/>
-      <c r="G51" s="29"/>
-      <c r="H51" s="30"/>
-      <c r="I51" s="30"/>
-      <c r="J51" s="31"/>
-      <c r="K51" s="35"/>
-      <c r="L51" s="36"/>
+      <c r="G51" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="H51" s="30">
+        <v>27</v>
+      </c>
+      <c r="I51" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J51" s="31" t="s">
+        <v>192</v>
+      </c>
+      <c r="K51" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L51" s="36" t="s">
+        <v>32</v>
+      </c>
       <c r="M51" s="39"/>
-      <c r="N51" s="39"/>
+      <c r="N51" s="39" t="s">
+        <v>64</v>
+      </c>
       <c r="O51" s="38"/>
-      <c r="P51" s="37"/>
-      <c r="Q51" s="1"/>
-      <c r="R51" s="13"/>
-      <c r="S51" s="13"/>
-      <c r="T51" s="13"/>
-      <c r="U51" s="2"/>
-    </row>
-    <row r="52" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="21"/>
-      <c r="B52" s="22"/>
-      <c r="C52" s="23"/>
-      <c r="D52" s="24"/>
+      <c r="P51" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q51" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="R51" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="S51" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="T51" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="U51" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="V51" s="5"/>
+    </row>
+    <row r="52" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C52" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D52" s="45" t="s">
+        <v>205</v>
+      </c>
       <c r="E52" s="25"/>
       <c r="F52" s="26"/>
-      <c r="G52" s="29"/>
-      <c r="H52" s="30"/>
-      <c r="I52" s="30"/>
-      <c r="J52" s="31"/>
-      <c r="K52" s="35"/>
-      <c r="L52" s="36"/>
+      <c r="G52" s="29" t="s">
+        <v>210</v>
+      </c>
+      <c r="H52" s="30">
+        <v>28</v>
+      </c>
+      <c r="I52" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J52" s="31" t="s">
+        <v>211</v>
+      </c>
+      <c r="K52" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="L52" s="36" t="s">
+        <v>32</v>
+      </c>
       <c r="M52" s="39"/>
-      <c r="N52" s="39"/>
+      <c r="N52" s="39" t="s">
+        <v>64</v>
+      </c>
       <c r="O52" s="38"/>
-      <c r="P52" s="37"/>
-      <c r="Q52" s="1"/>
-      <c r="R52" s="13"/>
-      <c r="S52" s="13"/>
-      <c r="T52" s="13"/>
-      <c r="U52" s="2"/>
-    </row>
-    <row r="53" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="21"/>
-      <c r="B53" s="22"/>
-      <c r="C53" s="23"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="26"/>
-      <c r="G53" s="29"/>
-      <c r="H53" s="30"/>
-      <c r="I53" s="30"/>
-      <c r="J53" s="31"/>
-      <c r="K53" s="35"/>
-      <c r="L53" s="36"/>
-      <c r="M53" s="39"/>
-      <c r="N53" s="39"/>
-      <c r="O53" s="38"/>
-      <c r="P53" s="37"/>
-      <c r="Q53" s="1"/>
-      <c r="R53" s="13"/>
-      <c r="S53" s="13"/>
-      <c r="T53" s="13"/>
-      <c r="U53" s="2"/>
-    </row>
-    <row r="54" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="21"/>
-      <c r="B54" s="22"/>
-      <c r="C54" s="23"/>
-      <c r="D54" s="24"/>
+      <c r="P52" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q52" s="1">
+        <v>6</v>
+      </c>
+      <c r="R52" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="S52" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="T52" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="U52" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="V52" s="5"/>
+    </row>
+    <row r="53" spans="1:22" s="88" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="72" t="s">
+        <v>67</v>
+      </c>
+      <c r="B53" s="73" t="s">
+        <v>90</v>
+      </c>
+      <c r="C53" s="74" t="s">
+        <v>91</v>
+      </c>
+      <c r="D53" s="77" t="s">
+        <v>205</v>
+      </c>
+      <c r="E53" s="75"/>
+      <c r="F53" s="76"/>
+      <c r="G53" s="77" t="s">
+        <v>226</v>
+      </c>
+      <c r="H53" s="78">
+        <v>29</v>
+      </c>
+      <c r="I53" s="78" t="s">
+        <v>20</v>
+      </c>
+      <c r="J53" s="79" t="s">
+        <v>232</v>
+      </c>
+      <c r="K53" s="80" t="s">
+        <v>70</v>
+      </c>
+      <c r="L53" s="81" t="s">
+        <v>32</v>
+      </c>
+      <c r="M53" s="82"/>
+      <c r="N53" s="82" t="s">
+        <v>64</v>
+      </c>
+      <c r="O53" s="83"/>
+      <c r="P53" s="84" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q53" s="88" t="s">
+        <v>227</v>
+      </c>
+      <c r="R53" s="88" t="s">
+        <v>197</v>
+      </c>
+      <c r="S53" s="88" t="s">
+        <v>228</v>
+      </c>
+      <c r="T53" s="88" t="s">
+        <v>229</v>
+      </c>
+      <c r="U53" s="87" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B54" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C54" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D54" s="20" t="s">
+        <v>99</v>
+      </c>
       <c r="E54" s="25"/>
       <c r="F54" s="26"/>
-      <c r="G54" s="29"/>
-      <c r="H54" s="30"/>
-      <c r="I54" s="30"/>
-      <c r="J54" s="31"/>
-      <c r="K54" s="35"/>
-      <c r="L54" s="36"/>
+      <c r="G54" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="H54" s="30">
+        <v>30</v>
+      </c>
+      <c r="I54" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J54" s="31" t="s">
+        <v>194</v>
+      </c>
+      <c r="K54" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="L54" s="36" t="s">
+        <v>33</v>
+      </c>
       <c r="M54" s="39"/>
       <c r="N54" s="39"/>
       <c r="O54" s="38"/>
-      <c r="P54" s="37"/>
+      <c r="P54" s="37" t="s">
+        <v>19</v>
+      </c>
       <c r="Q54" s="1"/>
       <c r="R54" s="13"/>
       <c r="S54" s="13"/>
       <c r="T54" s="13"/>
       <c r="U54" s="2"/>
-    </row>
-    <row r="55" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="21"/>
-      <c r="B55" s="22"/>
-      <c r="C55" s="23"/>
-      <c r="D55" s="24"/>
+      <c r="V54" s="5"/>
+    </row>
+    <row r="55" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C55" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D55" s="20" t="s">
+        <v>99</v>
+      </c>
       <c r="E55" s="25"/>
       <c r="F55" s="26"/>
-      <c r="G55" s="29"/>
-      <c r="H55" s="30"/>
-      <c r="I55" s="30"/>
-      <c r="J55" s="31"/>
-      <c r="K55" s="35"/>
-      <c r="L55" s="36"/>
+      <c r="G55" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="H55" s="30">
+        <v>31</v>
+      </c>
+      <c r="I55" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J55" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="K55" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="L55" s="36" t="s">
+        <v>32</v>
+      </c>
       <c r="M55" s="39"/>
-      <c r="N55" s="39"/>
+      <c r="N55" s="39" t="s">
+        <v>23</v>
+      </c>
       <c r="O55" s="38"/>
-      <c r="P55" s="37"/>
-      <c r="Q55" s="1"/>
-      <c r="R55" s="13"/>
-      <c r="S55" s="13"/>
-      <c r="T55" s="13"/>
-      <c r="U55" s="2"/>
-    </row>
-    <row r="56" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="21"/>
-      <c r="B56" s="22"/>
-      <c r="C56" s="23"/>
+      <c r="P55" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q55" s="1">
+        <v>6</v>
+      </c>
+      <c r="R55" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="S55" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="T55" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="U55" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="V55" s="5"/>
+    </row>
+    <row r="56" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B56" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C56" s="20" t="s">
+        <v>91</v>
+      </c>
       <c r="D56" s="24"/>
       <c r="E56" s="25"/>
       <c r="F56" s="26"/>
-      <c r="G56" s="29"/>
-      <c r="H56" s="30"/>
-      <c r="I56" s="30"/>
-      <c r="J56" s="31"/>
-      <c r="K56" s="35"/>
-      <c r="L56" s="36"/>
+      <c r="G56" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="H56" s="30">
+        <v>32</v>
+      </c>
+      <c r="I56" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J56" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="K56" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="L56" s="36" t="s">
+        <v>32</v>
+      </c>
       <c r="M56" s="39"/>
-      <c r="N56" s="39"/>
+      <c r="N56" s="39" t="s">
+        <v>63</v>
+      </c>
       <c r="O56" s="38"/>
-      <c r="P56" s="37"/>
-      <c r="Q56" s="1"/>
-      <c r="R56" s="13"/>
-      <c r="S56" s="13"/>
-      <c r="T56" s="13"/>
-      <c r="U56" s="2"/>
-    </row>
-    <row r="57" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P56" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q56" s="1">
+        <v>6</v>
+      </c>
+      <c r="R56" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="S56" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="T56" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="U56" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="21"/>
       <c r="B57" s="22"/>
       <c r="C57" s="23"/>
@@ -4091,7 +4401,7 @@
       <c r="T57" s="13"/>
       <c r="U57" s="2"/>
     </row>
-    <row r="58" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="21"/>
       <c r="B58" s="22"/>
       <c r="C58" s="23"/>
@@ -4114,7 +4424,7 @@
       <c r="T58" s="13"/>
       <c r="U58" s="2"/>
     </row>
-    <row r="59" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="21"/>
       <c r="B59" s="22"/>
       <c r="C59" s="23"/>
@@ -4137,7 +4447,7 @@
       <c r="T59" s="13"/>
       <c r="U59" s="2"/>
     </row>
-    <row r="60" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="21"/>
       <c r="B60" s="22"/>
       <c r="C60" s="23"/>
@@ -4160,7 +4470,7 @@
       <c r="T60" s="13"/>
       <c r="U60" s="2"/>
     </row>
-    <row r="61" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="21"/>
       <c r="B61" s="22"/>
       <c r="C61" s="23"/>
@@ -4183,7 +4493,7 @@
       <c r="T61" s="13"/>
       <c r="U61" s="2"/>
     </row>
-    <row r="62" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="21"/>
       <c r="B62" s="22"/>
       <c r="C62" s="23"/>
@@ -4206,7 +4516,7 @@
       <c r="T62" s="13"/>
       <c r="U62" s="2"/>
     </row>
-    <row r="63" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="21"/>
       <c r="B63" s="22"/>
       <c r="C63" s="23"/>
@@ -4229,7 +4539,7 @@
       <c r="T63" s="13"/>
       <c r="U63" s="2"/>
     </row>
-    <row r="64" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="21"/>
       <c r="B64" s="22"/>
       <c r="C64" s="23"/>
@@ -4252,7 +4562,7 @@
       <c r="T64" s="13"/>
       <c r="U64" s="2"/>
     </row>
-    <row r="65" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="21"/>
       <c r="B65" s="22"/>
       <c r="C65" s="23"/>
@@ -4275,7 +4585,7 @@
       <c r="T65" s="13"/>
       <c r="U65" s="2"/>
     </row>
-    <row r="66" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="21"/>
       <c r="B66" s="22"/>
       <c r="C66" s="23"/>
@@ -4298,7 +4608,7 @@
       <c r="T66" s="13"/>
       <c r="U66" s="2"/>
     </row>
-    <row r="67" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="21"/>
       <c r="B67" s="22"/>
       <c r="C67" s="23"/>
@@ -4321,7 +4631,7 @@
       <c r="T67" s="13"/>
       <c r="U67" s="2"/>
     </row>
-    <row r="68" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="21"/>
       <c r="B68" s="22"/>
       <c r="C68" s="23"/>
@@ -4344,7 +4654,7 @@
       <c r="T68" s="13"/>
       <c r="U68" s="2"/>
     </row>
-    <row r="69" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="21"/>
       <c r="B69" s="22"/>
       <c r="C69" s="23"/>
@@ -4367,7 +4677,7 @@
       <c r="T69" s="13"/>
       <c r="U69" s="2"/>
     </row>
-    <row r="70" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="21"/>
       <c r="B70" s="22"/>
       <c r="C70" s="23"/>
@@ -4390,7 +4700,7 @@
       <c r="T70" s="13"/>
       <c r="U70" s="2"/>
     </row>
-    <row r="71" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="21"/>
       <c r="B71" s="22"/>
       <c r="C71" s="23"/>
@@ -4413,7 +4723,7 @@
       <c r="T71" s="13"/>
       <c r="U71" s="2"/>
     </row>
-    <row r="72" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="21"/>
       <c r="B72" s="22"/>
       <c r="C72" s="23"/>
@@ -4436,7 +4746,7 @@
       <c r="T72" s="13"/>
       <c r="U72" s="2"/>
     </row>
-    <row r="73" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="21"/>
       <c r="B73" s="22"/>
       <c r="C73" s="23"/>
@@ -4459,7 +4769,7 @@
       <c r="T73" s="13"/>
       <c r="U73" s="2"/>
     </row>
-    <row r="74" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="21"/>
       <c r="B74" s="22"/>
       <c r="C74" s="23"/>
@@ -4482,7 +4792,7 @@
       <c r="T74" s="13"/>
       <c r="U74" s="2"/>
     </row>
-    <row r="75" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="21"/>
       <c r="B75" s="22"/>
       <c r="C75" s="23"/>
@@ -4505,7 +4815,7 @@
       <c r="T75" s="13"/>
       <c r="U75" s="2"/>
     </row>
-    <row r="76" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="21"/>
       <c r="B76" s="22"/>
       <c r="C76" s="23"/>
@@ -4528,7 +4838,7 @@
       <c r="T76" s="13"/>
       <c r="U76" s="2"/>
     </row>
-    <row r="77" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="21"/>
       <c r="B77" s="22"/>
       <c r="C77" s="23"/>
@@ -4551,7 +4861,7 @@
       <c r="T77" s="13"/>
       <c r="U77" s="2"/>
     </row>
-    <row r="78" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="21"/>
       <c r="B78" s="22"/>
       <c r="C78" s="23"/>
@@ -4574,7 +4884,7 @@
       <c r="T78" s="13"/>
       <c r="U78" s="2"/>
     </row>
-    <row r="79" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="21"/>
       <c r="B79" s="22"/>
       <c r="C79" s="23"/>
@@ -4597,7 +4907,7 @@
       <c r="T79" s="13"/>
       <c r="U79" s="2"/>
     </row>
-    <row r="80" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="21"/>
       <c r="B80" s="22"/>
       <c r="C80" s="23"/>
@@ -4620,7 +4930,7 @@
       <c r="T80" s="13"/>
       <c r="U80" s="2"/>
     </row>
-    <row r="81" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="21"/>
       <c r="B81" s="22"/>
       <c r="C81" s="23"/>
@@ -4643,7 +4953,7 @@
       <c r="T81" s="13"/>
       <c r="U81" s="2"/>
     </row>
-    <row r="82" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="21"/>
       <c r="B82" s="22"/>
       <c r="C82" s="23"/>
@@ -4666,7 +4976,7 @@
       <c r="T82" s="13"/>
       <c r="U82" s="2"/>
     </row>
-    <row r="83" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="21"/>
       <c r="B83" s="22"/>
       <c r="C83" s="23"/>
@@ -4689,7 +4999,7 @@
       <c r="T83" s="13"/>
       <c r="U83" s="2"/>
     </row>
-    <row r="84" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="21"/>
       <c r="B84" s="22"/>
       <c r="C84" s="23"/>
@@ -4712,7 +5022,7 @@
       <c r="T84" s="13"/>
       <c r="U84" s="2"/>
     </row>
-    <row r="85" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="21"/>
       <c r="B85" s="22"/>
       <c r="C85" s="23"/>
@@ -4735,7 +5045,7 @@
       <c r="T85" s="13"/>
       <c r="U85" s="2"/>
     </row>
-    <row r="86" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="21"/>
       <c r="B86" s="22"/>
       <c r="C86" s="23"/>
@@ -4758,7 +5068,7 @@
       <c r="T86" s="13"/>
       <c r="U86" s="2"/>
     </row>
-    <row r="87" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="21"/>
       <c r="B87" s="22"/>
       <c r="C87" s="23"/>
@@ -4781,7 +5091,7 @@
       <c r="T87" s="13"/>
       <c r="U87" s="2"/>
     </row>
-    <row r="88" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="21"/>
       <c r="B88" s="22"/>
       <c r="C88" s="23"/>
@@ -4804,7 +5114,7 @@
       <c r="T88" s="13"/>
       <c r="U88" s="2"/>
     </row>
-    <row r="89" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="21"/>
       <c r="B89" s="22"/>
       <c r="C89" s="23"/>
@@ -4827,7 +5137,7 @@
       <c r="T89" s="13"/>
       <c r="U89" s="2"/>
     </row>
-    <row r="90" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="21"/>
       <c r="B90" s="22"/>
       <c r="C90" s="23"/>
@@ -4850,7 +5160,7 @@
       <c r="T90" s="13"/>
       <c r="U90" s="2"/>
     </row>
-    <row r="91" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="21"/>
       <c r="B91" s="22"/>
       <c r="C91" s="23"/>
@@ -4873,7 +5183,7 @@
       <c r="T91" s="13"/>
       <c r="U91" s="2"/>
     </row>
-    <row r="92" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="21"/>
       <c r="B92" s="22"/>
       <c r="C92" s="23"/>
@@ -4896,7 +5206,7 @@
       <c r="T92" s="13"/>
       <c r="U92" s="2"/>
     </row>
-    <row r="93" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="21"/>
       <c r="B93" s="22"/>
       <c r="C93" s="23"/>
@@ -4919,8 +5229,169 @@
       <c r="T93" s="13"/>
       <c r="U93" s="2"/>
     </row>
+    <row r="94" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="21"/>
+      <c r="B94" s="22"/>
+      <c r="C94" s="23"/>
+      <c r="D94" s="24"/>
+      <c r="E94" s="25"/>
+      <c r="F94" s="26"/>
+      <c r="G94" s="29"/>
+      <c r="H94" s="30"/>
+      <c r="I94" s="30"/>
+      <c r="J94" s="31"/>
+      <c r="K94" s="35"/>
+      <c r="L94" s="36"/>
+      <c r="M94" s="39"/>
+      <c r="N94" s="39"/>
+      <c r="O94" s="38"/>
+      <c r="P94" s="37"/>
+      <c r="Q94" s="1"/>
+      <c r="R94" s="13"/>
+      <c r="S94" s="13"/>
+      <c r="T94" s="13"/>
+      <c r="U94" s="2"/>
+    </row>
+    <row r="95" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="21"/>
+      <c r="B95" s="22"/>
+      <c r="C95" s="23"/>
+      <c r="D95" s="24"/>
+      <c r="E95" s="25"/>
+      <c r="F95" s="26"/>
+      <c r="G95" s="29"/>
+      <c r="H95" s="30"/>
+      <c r="I95" s="30"/>
+      <c r="J95" s="31"/>
+      <c r="K95" s="35"/>
+      <c r="L95" s="36"/>
+      <c r="M95" s="39"/>
+      <c r="N95" s="39"/>
+      <c r="O95" s="38"/>
+      <c r="P95" s="37"/>
+      <c r="Q95" s="1"/>
+      <c r="R95" s="13"/>
+      <c r="S95" s="13"/>
+      <c r="T95" s="13"/>
+      <c r="U95" s="2"/>
+    </row>
+    <row r="96" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="21"/>
+      <c r="B96" s="22"/>
+      <c r="C96" s="23"/>
+      <c r="D96" s="24"/>
+      <c r="E96" s="25"/>
+      <c r="F96" s="26"/>
+      <c r="G96" s="29"/>
+      <c r="H96" s="30"/>
+      <c r="I96" s="30"/>
+      <c r="J96" s="31"/>
+      <c r="K96" s="35"/>
+      <c r="L96" s="36"/>
+      <c r="M96" s="39"/>
+      <c r="N96" s="39"/>
+      <c r="O96" s="38"/>
+      <c r="P96" s="37"/>
+      <c r="Q96" s="1"/>
+      <c r="R96" s="13"/>
+      <c r="S96" s="13"/>
+      <c r="T96" s="13"/>
+      <c r="U96" s="2"/>
+    </row>
+    <row r="97" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="21"/>
+      <c r="B97" s="22"/>
+      <c r="C97" s="23"/>
+      <c r="D97" s="24"/>
+      <c r="E97" s="25"/>
+      <c r="F97" s="26"/>
+      <c r="G97" s="29"/>
+      <c r="H97" s="30"/>
+      <c r="I97" s="30"/>
+      <c r="J97" s="31"/>
+      <c r="K97" s="35"/>
+      <c r="L97" s="36"/>
+      <c r="M97" s="39"/>
+      <c r="N97" s="39"/>
+      <c r="O97" s="38"/>
+      <c r="P97" s="37"/>
+      <c r="Q97" s="1"/>
+      <c r="R97" s="13"/>
+      <c r="S97" s="13"/>
+      <c r="T97" s="13"/>
+      <c r="U97" s="2"/>
+    </row>
+    <row r="98" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="21"/>
+      <c r="B98" s="22"/>
+      <c r="C98" s="23"/>
+      <c r="D98" s="24"/>
+      <c r="E98" s="25"/>
+      <c r="F98" s="26"/>
+      <c r="G98" s="29"/>
+      <c r="H98" s="30"/>
+      <c r="I98" s="30"/>
+      <c r="J98" s="31"/>
+      <c r="K98" s="35"/>
+      <c r="L98" s="36"/>
+      <c r="M98" s="39"/>
+      <c r="N98" s="39"/>
+      <c r="O98" s="38"/>
+      <c r="P98" s="37"/>
+      <c r="Q98" s="1"/>
+      <c r="R98" s="13"/>
+      <c r="S98" s="13"/>
+      <c r="T98" s="13"/>
+      <c r="U98" s="2"/>
+    </row>
+    <row r="99" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="21"/>
+      <c r="B99" s="22"/>
+      <c r="C99" s="23"/>
+      <c r="D99" s="24"/>
+      <c r="E99" s="25"/>
+      <c r="F99" s="26"/>
+      <c r="G99" s="29"/>
+      <c r="H99" s="30"/>
+      <c r="I99" s="30"/>
+      <c r="J99" s="31"/>
+      <c r="K99" s="35"/>
+      <c r="L99" s="36"/>
+      <c r="M99" s="39"/>
+      <c r="N99" s="39"/>
+      <c r="O99" s="38"/>
+      <c r="P99" s="37"/>
+      <c r="Q99" s="1"/>
+      <c r="R99" s="13"/>
+      <c r="S99" s="13"/>
+      <c r="T99" s="13"/>
+      <c r="U99" s="2"/>
+    </row>
+    <row r="100" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="21"/>
+      <c r="B100" s="22"/>
+      <c r="C100" s="23"/>
+      <c r="D100" s="24"/>
+      <c r="E100" s="25"/>
+      <c r="F100" s="26"/>
+      <c r="G100" s="29"/>
+      <c r="H100" s="30"/>
+      <c r="I100" s="30"/>
+      <c r="J100" s="31"/>
+      <c r="K100" s="35"/>
+      <c r="L100" s="36"/>
+      <c r="M100" s="39"/>
+      <c r="N100" s="39"/>
+      <c r="O100" s="38"/>
+      <c r="P100" s="37"/>
+      <c r="Q100" s="1"/>
+      <c r="R100" s="13"/>
+      <c r="S100" s="13"/>
+      <c r="T100" s="13"/>
+      <c r="U100" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="P1:P93">
+  <autoFilter ref="P1:P100">
     <filterColumn colId="0">
       <filters>
         <filter val="SI"/>
@@ -4928,6 +5399,11 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="U1:U2"/>
@@ -4943,52 +5419,83 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="M1:N1"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="12">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$D$2:$D$5</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A93</xm:sqref>
+          <xm:sqref>A3:A22 A24:A100</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>K3:K93</xm:sqref>
+          <xm:sqref>K3:K22 K24:K100</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$F$2:$F$6</xm:f>
           </x14:formula1>
-          <xm:sqref>L3:L93</xm:sqref>
+          <xm:sqref>L3:L22 L24:L100</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$G$2:$G$3</xm:f>
           </x14:formula1>
-          <xm:sqref>P3:P93</xm:sqref>
+          <xm:sqref>P3:P22 P24:P100</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$C$2:$C$39</xm:f>
           </x14:formula1>
-          <xm:sqref>N3:N93</xm:sqref>
+          <xm:sqref>N3:N22 N24:N100</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$B$2:$B$14</xm:f>
           </x14:formula1>
-          <xm:sqref>M3:M93</xm:sqref>
+          <xm:sqref>M3:M22 M24:M100</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]DATOS!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>N23</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]DATOS!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>M23</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]DATOS!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>P23</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]DATOS!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>L23</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]DATOS!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>K23</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]DATOS!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>A23</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Adición de información de motores
Adición de información de motores
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion09/ESCALETA FINAL CN_11_09_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion09/ESCALETA FINAL CN_11_09_CO.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="237">
   <si>
     <t>Asignatura</t>
   </si>
@@ -678,9 +678,6 @@
     <t>Animación se encuentra en http://hispanicasaber.planetasaber.com/encyclopedia/default.asp?idpack=5&amp;idpil=AN001056&amp;ruta=Buscador</t>
   </si>
   <si>
-    <t>Recurso F12-01</t>
-  </si>
-  <si>
     <t>Actividades sobre La electroquímica</t>
   </si>
   <si>
@@ -808,6 +805,21 @@
   </si>
   <si>
     <t>Actividad que guía el trabajo colaborativo sobre la investigación de las cualidades del champú</t>
+  </si>
+  <si>
+    <t>Recurso M101A-02</t>
+  </si>
+  <si>
+    <t>Recursos adicionales 01</t>
+  </si>
+  <si>
+    <t>Video como media principal - 01</t>
+  </si>
+  <si>
+    <t>RF_01_02_CO</t>
+  </si>
+  <si>
+    <t>Recurso F6-03</t>
   </si>
 </sst>
 </file>
@@ -1300,30 +1312,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1384,6 +1372,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1680,11 +1692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:W100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P49" sqref="P49"/>
+    <sheetView tabSelected="1" topLeftCell="K16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1712,94 +1723,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="G1" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="H1" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="I1" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="47" t="s">
+      <c r="J1" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="51" t="s">
+      <c r="K1" s="88" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="49" t="s">
+      <c r="L1" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="53" t="s">
+      <c r="M1" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="54"/>
-      <c r="O1" s="47" t="s">
+      <c r="N1" s="91"/>
+      <c r="O1" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="47" t="s">
+      <c r="P1" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="47" t="s">
+      <c r="Q1" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="47" t="s">
+      <c r="R1" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="47" t="s">
+      <c r="S1" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="47" t="s">
+      <c r="T1" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="47" t="s">
+      <c r="U1" s="84" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="50"/>
+      <c r="A2" s="85"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="87"/>
       <c r="M2" s="46" t="s">
         <v>87</v>
       </c>
       <c r="N2" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="48"/>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
-      <c r="U2" s="48"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="85"/>
+      <c r="S2" s="85"/>
+      <c r="T2" s="85"/>
+      <c r="U2" s="85"/>
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -2016,59 +2027,59 @@
         <v>154</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="88" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="72" t="s">
+    <row r="8" spans="1:21" s="80" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="74" t="s">
+      <c r="C8" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="74" t="s">
+      <c r="D8" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="E8" s="75"/>
-      <c r="F8" s="76"/>
-      <c r="G8" s="77" t="s">
+      <c r="E8" s="67"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="69" t="s">
+        <v>213</v>
+      </c>
+      <c r="H8" s="70">
+        <v>3</v>
+      </c>
+      <c r="I8" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="71" t="s">
         <v>214</v>
       </c>
-      <c r="H8" s="78">
-        <v>3</v>
-      </c>
-      <c r="I8" s="78" t="s">
+      <c r="K8" s="72" t="s">
+        <v>69</v>
+      </c>
+      <c r="L8" s="73"/>
+      <c r="M8" s="74"/>
+      <c r="N8" s="74"/>
+      <c r="O8" s="75" t="s">
+        <v>215</v>
+      </c>
+      <c r="P8" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="79" t="s">
-        <v>215</v>
-      </c>
-      <c r="K8" s="80" t="s">
-        <v>69</v>
-      </c>
-      <c r="L8" s="81"/>
-      <c r="M8" s="82"/>
-      <c r="N8" s="82"/>
-      <c r="O8" s="83" t="s">
+      <c r="Q8" s="77">
+        <v>6</v>
+      </c>
+      <c r="R8" s="78" t="s">
+        <v>152</v>
+      </c>
+      <c r="S8" s="78" t="s">
         <v>216</v>
       </c>
-      <c r="P8" s="84" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q8" s="85">
-        <v>6</v>
-      </c>
-      <c r="R8" s="86" t="s">
-        <v>152</v>
-      </c>
-      <c r="S8" s="86" t="s">
+      <c r="T8" s="78" t="s">
         <v>217</v>
       </c>
-      <c r="T8" s="86" t="s">
+      <c r="U8" s="79" t="s">
         <v>218</v>
-      </c>
-      <c r="U8" s="87" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2172,9 +2183,7 @@
       <c r="L11" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="M11" s="39" t="s">
-        <v>36</v>
-      </c>
+      <c r="M11" s="39"/>
       <c r="N11" s="39"/>
       <c r="O11" s="38"/>
       <c r="P11" s="37"/>
@@ -2182,60 +2191,72 @@
         <v>6</v>
       </c>
       <c r="R11" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="S11" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="T11" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" s="80" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="64" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" s="66" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" s="67"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="69" t="s">
+        <v>219</v>
+      </c>
+      <c r="H12" s="70">
+        <v>5</v>
+      </c>
+      <c r="I12" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="71" t="s">
+        <v>220</v>
+      </c>
+      <c r="K12" s="72" t="s">
+        <v>69</v>
+      </c>
+      <c r="L12" s="73" t="s">
+        <v>31</v>
+      </c>
+      <c r="M12" s="74" t="s">
+        <v>36</v>
+      </c>
+      <c r="N12" s="74"/>
+      <c r="O12" s="75"/>
+      <c r="P12" s="76"/>
+      <c r="Q12" s="77">
+        <v>6</v>
+      </c>
+      <c r="R12" s="78" t="s">
         <v>157</v>
       </c>
-      <c r="S11" s="13" t="s">
+      <c r="S12" s="78" t="s">
         <v>158</v>
       </c>
-      <c r="T11" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="U11" s="2" t="s">
+      <c r="T12" s="78" t="s">
+        <v>221</v>
+      </c>
+      <c r="U12" s="79" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" s="88" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="72" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="73" t="s">
-        <v>90</v>
-      </c>
-      <c r="C12" s="74" t="s">
-        <v>91</v>
-      </c>
-      <c r="D12" s="74" t="s">
-        <v>94</v>
-      </c>
-      <c r="E12" s="75"/>
-      <c r="F12" s="76"/>
-      <c r="G12" s="77" t="s">
-        <v>220</v>
-      </c>
-      <c r="H12" s="78">
-        <v>5</v>
-      </c>
-      <c r="I12" s="78" t="s">
-        <v>19</v>
-      </c>
-      <c r="J12" s="79" t="s">
-        <v>221</v>
-      </c>
-      <c r="K12" s="80" t="s">
-        <v>69</v>
-      </c>
-      <c r="L12" s="81" t="s">
-        <v>31</v>
-      </c>
-      <c r="M12" s="82"/>
-      <c r="N12" s="82"/>
-      <c r="O12" s="83"/>
-      <c r="P12" s="84"/>
-      <c r="Q12" s="85"/>
-      <c r="R12" s="86"/>
-      <c r="S12" s="86"/>
-      <c r="T12" s="86"/>
-      <c r="U12" s="87"/>
     </row>
     <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
@@ -2347,13 +2368,13 @@
         <v>19</v>
       </c>
       <c r="Q15" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="R15" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="R15" s="13" t="s">
+      <c r="S15" s="13" t="s">
         <v>197</v>
-      </c>
-      <c r="S15" s="13" t="s">
-        <v>198</v>
       </c>
       <c r="T15" s="13" t="s">
         <v>134</v>
@@ -2467,13 +2488,13 @@
         <v>19</v>
       </c>
       <c r="Q17" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="R17" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="R17" s="13" t="s">
+      <c r="S17" s="13" t="s">
         <v>197</v>
-      </c>
-      <c r="S17" s="13" t="s">
-        <v>198</v>
       </c>
       <c r="T17" s="13" t="s">
         <v>137</v>
@@ -2528,16 +2549,16 @@
         <v>19</v>
       </c>
       <c r="Q18" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="R18" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="R18" s="13" t="s">
+      <c r="S18" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="S18" s="13" t="s">
+      <c r="T18" s="13" t="s">
         <v>198</v>
-      </c>
-      <c r="T18" s="13" t="s">
-        <v>199</v>
       </c>
       <c r="U18" s="2" t="s">
         <v>164</v>
@@ -2588,16 +2609,16 @@
         <v>19</v>
       </c>
       <c r="Q19" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="R19" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="R19" s="13" t="s">
+      <c r="S19" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="S19" s="13" t="s">
-        <v>198</v>
-      </c>
       <c r="T19" s="13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="U19" s="2" t="s">
         <v>164</v>
@@ -2696,60 +2717,60 @@
         <v>154</v>
       </c>
     </row>
-    <row r="22" spans="1:23" s="88" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="72" t="s">
+    <row r="22" spans="1:23" s="80" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="B22" s="73" t="s">
+      <c r="B22" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="74" t="s">
+      <c r="C22" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="D22" s="74" t="s">
+      <c r="D22" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="E22" s="75"/>
-      <c r="F22" s="76"/>
-      <c r="G22" s="77" t="s">
+      <c r="E22" s="67"/>
+      <c r="F22" s="68"/>
+      <c r="G22" s="69" t="s">
+        <v>222</v>
+      </c>
+      <c r="H22" s="70">
+        <v>12</v>
+      </c>
+      <c r="I22" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" s="71" t="s">
         <v>223</v>
       </c>
-      <c r="H22" s="78">
-        <v>12</v>
-      </c>
-      <c r="I22" s="78" t="s">
+      <c r="K22" s="72" t="s">
+        <v>69</v>
+      </c>
+      <c r="L22" s="73" t="s">
+        <v>31</v>
+      </c>
+      <c r="M22" s="74" t="s">
+        <v>46</v>
+      </c>
+      <c r="N22" s="74"/>
+      <c r="O22" s="75"/>
+      <c r="P22" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="J22" s="79" t="s">
+      <c r="Q22" s="80">
+        <v>6</v>
+      </c>
+      <c r="R22" s="80" t="s">
+        <v>157</v>
+      </c>
+      <c r="S22" s="80" t="s">
+        <v>158</v>
+      </c>
+      <c r="T22" s="81" t="s">
         <v>224</v>
       </c>
-      <c r="K22" s="80" t="s">
-        <v>69</v>
-      </c>
-      <c r="L22" s="81" t="s">
-        <v>31</v>
-      </c>
-      <c r="M22" s="82" t="s">
-        <v>46</v>
-      </c>
-      <c r="N22" s="82"/>
-      <c r="O22" s="83"/>
-      <c r="P22" s="84" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q22" s="88">
-        <v>6</v>
-      </c>
-      <c r="R22" s="88" t="s">
-        <v>157</v>
-      </c>
-      <c r="S22" s="88" t="s">
-        <v>158</v>
-      </c>
-      <c r="T22" s="89" t="s">
-        <v>225</v>
-      </c>
-      <c r="U22" s="88" t="s">
+      <c r="U22" s="80" t="s">
         <v>160</v>
       </c>
     </row>
@@ -2797,13 +2818,13 @@
         <v>19</v>
       </c>
       <c r="Q23" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="R23" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="R23" s="13" t="s">
+      <c r="S23" s="13" t="s">
         <v>197</v>
-      </c>
-      <c r="S23" s="13" t="s">
-        <v>198</v>
       </c>
       <c r="T23" s="13" t="s">
         <v>140</v>
@@ -2948,19 +2969,19 @@
       <c r="M27" s="39"/>
       <c r="N27" s="39"/>
       <c r="O27" s="38" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="P27" s="37" t="s">
         <v>19</v>
       </c>
       <c r="Q27" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="R27" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="R27" s="13" t="s">
+      <c r="S27" s="13" t="s">
         <v>197</v>
-      </c>
-      <c r="S27" s="13" t="s">
-        <v>198</v>
       </c>
       <c r="T27" s="13" t="s">
         <v>141</v>
@@ -3012,16 +3033,16 @@
         <v>19</v>
       </c>
       <c r="Q28" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="R28" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="R28" s="13" t="s">
+      <c r="S28" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="S28" s="13" t="s">
-        <v>198</v>
-      </c>
       <c r="T28" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="U28" s="2" t="s">
         <v>164</v>
@@ -3070,16 +3091,16 @@
         <v>19</v>
       </c>
       <c r="Q29" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="R29" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="R29" s="13" t="s">
+      <c r="S29" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="S29" s="13" t="s">
-        <v>198</v>
-      </c>
       <c r="T29" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="U29" s="2" t="s">
         <v>164</v>
@@ -3087,7 +3108,7 @@
       <c r="V29" s="5"/>
       <c r="W29" s="5"/>
     </row>
-    <row r="30" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>67</v>
       </c>
@@ -3122,7 +3143,7 @@
       <c r="T30" s="13"/>
       <c r="U30" s="2"/>
     </row>
-    <row r="31" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
         <v>67</v>
       </c>
@@ -3157,7 +3178,7 @@
       <c r="T31" s="13"/>
       <c r="U31" s="2"/>
     </row>
-    <row r="32" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
         <v>67</v>
       </c>
@@ -3192,7 +3213,7 @@
       <c r="T32" s="13"/>
       <c r="U32" s="2"/>
     </row>
-    <row r="33" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
         <v>67</v>
       </c>
@@ -3286,60 +3307,60 @@
         <v>154</v>
       </c>
     </row>
-    <row r="35" spans="1:22" s="88" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="72" t="s">
+    <row r="35" spans="1:22" s="80" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="73" t="s">
+      <c r="B35" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="C35" s="74" t="s">
+      <c r="C35" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="D35" s="74" t="s">
+      <c r="D35" s="66" t="s">
         <v>97</v>
       </c>
-      <c r="E35" s="75"/>
-      <c r="F35" s="76"/>
-      <c r="G35" s="77" t="s">
+      <c r="E35" s="67"/>
+      <c r="F35" s="68"/>
+      <c r="G35" s="69" t="s">
+        <v>229</v>
+      </c>
+      <c r="H35" s="70">
+        <v>18</v>
+      </c>
+      <c r="I35" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="J35" s="71" t="s">
         <v>230</v>
       </c>
-      <c r="H35" s="78">
-        <v>18</v>
-      </c>
-      <c r="I35" s="78" t="s">
+      <c r="K35" s="72" t="s">
+        <v>69</v>
+      </c>
+      <c r="L35" s="73" t="s">
+        <v>31</v>
+      </c>
+      <c r="M35" s="74" t="s">
+        <v>36</v>
+      </c>
+      <c r="N35" s="74"/>
+      <c r="O35" s="75"/>
+      <c r="P35" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="J35" s="79" t="s">
-        <v>231</v>
-      </c>
-      <c r="K35" s="80" t="s">
-        <v>69</v>
-      </c>
-      <c r="L35" s="81" t="s">
-        <v>31</v>
-      </c>
-      <c r="M35" s="82" t="s">
-        <v>36</v>
-      </c>
-      <c r="N35" s="82"/>
-      <c r="O35" s="83"/>
-      <c r="P35" s="84" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q35" s="85">
+      <c r="Q35" s="77">
         <v>6</v>
       </c>
-      <c r="R35" s="86" t="s">
+      <c r="R35" s="78" t="s">
         <v>157</v>
       </c>
-      <c r="S35" s="86" t="s">
+      <c r="S35" s="78" t="s">
         <v>158</v>
       </c>
-      <c r="T35" s="86" t="s">
-        <v>222</v>
-      </c>
-      <c r="U35" s="87" t="s">
+      <c r="T35" s="78" t="s">
+        <v>236</v>
+      </c>
+      <c r="U35" s="79" t="s">
         <v>160</v>
       </c>
     </row>
@@ -3383,13 +3404,13 @@
         <v>19</v>
       </c>
       <c r="Q36" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="R36" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="R36" s="13" t="s">
+      <c r="S36" s="13" t="s">
         <v>197</v>
-      </c>
-      <c r="S36" s="13" t="s">
-        <v>198</v>
       </c>
       <c r="T36" s="13" t="s">
         <v>144</v>
@@ -3439,13 +3460,13 @@
         <v>19</v>
       </c>
       <c r="Q37" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="R37" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="R37" s="13" t="s">
+      <c r="S37" s="13" t="s">
         <v>197</v>
-      </c>
-      <c r="S37" s="13" t="s">
-        <v>198</v>
       </c>
       <c r="T37" s="13" t="s">
         <v>145</v>
@@ -3497,13 +3518,13 @@
         <v>19</v>
       </c>
       <c r="Q38" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="R38" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="R38" s="13" t="s">
+      <c r="S38" s="13" t="s">
         <v>197</v>
-      </c>
-      <c r="S38" s="13" t="s">
-        <v>198</v>
       </c>
       <c r="T38" s="13" t="s">
         <v>146</v>
@@ -3788,9 +3809,7 @@
       <c r="L46" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="M46" s="39" t="s">
-        <v>44</v>
-      </c>
+      <c r="M46" s="39"/>
       <c r="N46" s="39"/>
       <c r="O46" s="38" t="s">
         <v>188</v>
@@ -3805,183 +3824,185 @@
         <v>157</v>
       </c>
       <c r="S46" s="13" t="s">
-        <v>158</v>
+        <v>233</v>
       </c>
       <c r="T46" s="13" t="s">
-        <v>189</v>
+        <v>234</v>
       </c>
       <c r="U46" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="47" spans="1:22" s="71" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="55" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" s="63" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="B47" s="56" t="s">
+      <c r="B47" s="48" t="s">
         <v>90</v>
       </c>
-      <c r="C47" s="57" t="s">
+      <c r="C47" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="D47" s="57" t="s">
+      <c r="D47" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="E47" s="58"/>
-      <c r="F47" s="59" t="s">
+      <c r="E47" s="50"/>
+      <c r="F47" s="51" t="s">
         <v>131</v>
       </c>
-      <c r="G47" s="60" t="s">
+      <c r="G47" s="52" t="s">
         <v>147</v>
       </c>
-      <c r="H47" s="61">
+      <c r="H47" s="53">
         <v>23</v>
       </c>
-      <c r="I47" s="61" t="s">
+      <c r="I47" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="J47" s="62" t="s">
+      <c r="J47" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="K47" s="63" t="s">
+      <c r="K47" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="L47" s="64" t="s">
+      <c r="L47" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="M47" s="65"/>
-      <c r="N47" s="65"/>
-      <c r="O47" s="66"/>
-      <c r="P47" s="67" t="s">
+      <c r="M47" s="57"/>
+      <c r="N47" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="O47" s="58"/>
+      <c r="P47" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="Q47" s="68" t="s">
+      <c r="Q47" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="R47" s="61" t="s">
         <v>196</v>
       </c>
-      <c r="R47" s="69" t="s">
+      <c r="S47" s="61" t="s">
         <v>197</v>
       </c>
-      <c r="S47" s="69" t="s">
-        <v>198</v>
-      </c>
-      <c r="T47" s="69" t="s">
-        <v>203</v>
-      </c>
-      <c r="U47" s="70" t="s">
+      <c r="T47" s="61" t="s">
+        <v>202</v>
+      </c>
+      <c r="U47" s="62" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="48" spans="1:22" s="71" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="55" t="s">
+    <row r="48" spans="1:22" s="63" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="B48" s="56" t="s">
+      <c r="B48" s="48" t="s">
         <v>90</v>
       </c>
-      <c r="C48" s="57" t="s">
+      <c r="C48" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="D48" s="57" t="s">
+      <c r="D48" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="E48" s="58"/>
-      <c r="F48" s="59" t="s">
+      <c r="E48" s="50"/>
+      <c r="F48" s="51" t="s">
         <v>131</v>
       </c>
-      <c r="G48" s="91" t="s">
+      <c r="G48" s="83" t="s">
         <v>184</v>
       </c>
-      <c r="H48" s="61">
+      <c r="H48" s="53">
         <v>24</v>
       </c>
-      <c r="I48" s="61" t="s">
+      <c r="I48" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="J48" s="62" t="s">
+      <c r="J48" s="54" t="s">
         <v>186</v>
       </c>
-      <c r="K48" s="63" t="s">
+      <c r="K48" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="L48" s="64" t="s">
+      <c r="L48" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="M48" s="65"/>
-      <c r="N48" s="65" t="s">
+      <c r="M48" s="57"/>
+      <c r="N48" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="O48" s="66"/>
-      <c r="P48" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q48" s="68">
+      <c r="O48" s="58"/>
+      <c r="P48" s="82" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q48" s="60">
         <v>6</v>
       </c>
-      <c r="R48" s="69" t="s">
+      <c r="R48" s="61" t="s">
         <v>152</v>
       </c>
-      <c r="S48" s="69" t="s">
+      <c r="S48" s="61" t="s">
         <v>153</v>
       </c>
-      <c r="T48" s="69" t="s">
+      <c r="T48" s="61" t="s">
         <v>185</v>
       </c>
-      <c r="U48" s="70" t="s">
+      <c r="U48" s="62" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="49" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="55" t="s">
+      <c r="A49" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="B49" s="56" t="s">
+      <c r="B49" s="48" t="s">
         <v>90</v>
       </c>
-      <c r="C49" s="57" t="s">
+      <c r="C49" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="D49" s="57" t="s">
+      <c r="D49" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="E49" s="58"/>
-      <c r="F49" s="59"/>
-      <c r="G49" s="60" t="s">
+      <c r="E49" s="50"/>
+      <c r="F49" s="51"/>
+      <c r="G49" s="52" t="s">
         <v>135</v>
       </c>
-      <c r="H49" s="61">
+      <c r="H49" s="53">
         <v>25</v>
       </c>
-      <c r="I49" s="61" t="s">
+      <c r="I49" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="J49" s="62" t="s">
-        <v>193</v>
-      </c>
-      <c r="K49" s="63" t="s">
+      <c r="J49" s="54" t="s">
+        <v>192</v>
+      </c>
+      <c r="K49" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="L49" s="64" t="s">
+      <c r="L49" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="M49" s="65"/>
-      <c r="N49" s="65"/>
-      <c r="O49" s="66"/>
-      <c r="P49" s="90" t="s">
+      <c r="M49" s="57"/>
+      <c r="N49" s="57"/>
+      <c r="O49" s="58"/>
+      <c r="P49" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="Q49" s="68" t="s">
+      <c r="Q49" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="R49" s="61" t="s">
         <v>196</v>
       </c>
-      <c r="R49" s="69" t="s">
+      <c r="S49" s="61" t="s">
         <v>197</v>
       </c>
-      <c r="S49" s="69" t="s">
-        <v>198</v>
-      </c>
-      <c r="T49" s="69" t="s">
+      <c r="T49" s="61" t="s">
         <v>135</v>
       </c>
-      <c r="U49" s="70" t="s">
+      <c r="U49" s="62" t="s">
         <v>164</v>
       </c>
       <c r="V49" s="5"/>
@@ -4013,7 +4034,7 @@
         <v>20</v>
       </c>
       <c r="J50" s="31" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K50" s="35" t="s">
         <v>69</v>
@@ -4039,7 +4060,7 @@
         <v>153</v>
       </c>
       <c r="T50" s="13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="U50" s="2" t="s">
         <v>154</v>
@@ -4057,7 +4078,7 @@
         <v>91</v>
       </c>
       <c r="D51" s="45" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E51" s="25"/>
       <c r="F51" s="26"/>
@@ -4071,7 +4092,7 @@
         <v>20</v>
       </c>
       <c r="J51" s="31" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K51" s="35" t="s">
         <v>70</v>
@@ -4088,16 +4109,16 @@
         <v>19</v>
       </c>
       <c r="Q51" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="R51" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="R51" s="13" t="s">
+      <c r="S51" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="S51" s="13" t="s">
-        <v>198</v>
-      </c>
       <c r="T51" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="U51" s="2" t="s">
         <v>164</v>
@@ -4115,12 +4136,12 @@
         <v>91</v>
       </c>
       <c r="D52" s="45" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E52" s="25"/>
       <c r="F52" s="26"/>
       <c r="G52" s="29" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H52" s="30">
         <v>28</v>
@@ -4129,7 +4150,7 @@
         <v>20</v>
       </c>
       <c r="J52" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K52" s="35" t="s">
         <v>69</v>
@@ -4155,67 +4176,67 @@
         <v>153</v>
       </c>
       <c r="T52" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="U52" s="2" t="s">
         <v>154</v>
       </c>
       <c r="V52" s="5"/>
     </row>
-    <row r="53" spans="1:22" s="88" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="72" t="s">
+    <row r="53" spans="1:22" s="80" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="B53" s="73" t="s">
+      <c r="B53" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="C53" s="74" t="s">
+      <c r="C53" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="D53" s="77" t="s">
-        <v>205</v>
-      </c>
-      <c r="E53" s="75"/>
-      <c r="F53" s="76"/>
-      <c r="G53" s="77" t="s">
+      <c r="D53" s="69" t="s">
+        <v>204</v>
+      </c>
+      <c r="E53" s="67"/>
+      <c r="F53" s="68"/>
+      <c r="G53" s="69" t="s">
+        <v>225</v>
+      </c>
+      <c r="H53" s="70">
+        <v>29</v>
+      </c>
+      <c r="I53" s="70" t="s">
+        <v>20</v>
+      </c>
+      <c r="J53" s="71" t="s">
+        <v>231</v>
+      </c>
+      <c r="K53" s="72" t="s">
+        <v>70</v>
+      </c>
+      <c r="L53" s="73" t="s">
+        <v>32</v>
+      </c>
+      <c r="M53" s="74"/>
+      <c r="N53" s="74" t="s">
+        <v>64</v>
+      </c>
+      <c r="O53" s="75"/>
+      <c r="P53" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q53" s="80" t="s">
         <v>226</v>
       </c>
-      <c r="H53" s="78">
-        <v>29</v>
-      </c>
-      <c r="I53" s="78" t="s">
-        <v>20</v>
-      </c>
-      <c r="J53" s="79" t="s">
-        <v>232</v>
-      </c>
-      <c r="K53" s="80" t="s">
-        <v>70</v>
-      </c>
-      <c r="L53" s="81" t="s">
-        <v>32</v>
-      </c>
-      <c r="M53" s="82"/>
-      <c r="N53" s="82" t="s">
-        <v>64</v>
-      </c>
-      <c r="O53" s="83"/>
-      <c r="P53" s="84" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q53" s="88" t="s">
+      <c r="R53" s="80" t="s">
+        <v>196</v>
+      </c>
+      <c r="S53" s="80" t="s">
         <v>227</v>
       </c>
-      <c r="R53" s="88" t="s">
-        <v>197</v>
-      </c>
-      <c r="S53" s="88" t="s">
+      <c r="T53" s="80" t="s">
         <v>228</v>
       </c>
-      <c r="T53" s="88" t="s">
-        <v>229</v>
-      </c>
-      <c r="U53" s="87" t="s">
+      <c r="U53" s="79" t="s">
         <v>164</v>
       </c>
     </row>
@@ -4244,7 +4265,7 @@
         <v>20</v>
       </c>
       <c r="J54" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K54" s="35" t="s">
         <v>69</v>
@@ -4290,7 +4311,7 @@
         <v>20</v>
       </c>
       <c r="J55" s="31" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K55" s="35" t="s">
         <v>69</v>
@@ -4316,7 +4337,7 @@
         <v>153</v>
       </c>
       <c r="T55" s="13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="U55" s="2" t="s">
         <v>154</v>
@@ -4337,7 +4358,7 @@
       <c r="E56" s="25"/>
       <c r="F56" s="26"/>
       <c r="G56" s="29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H56" s="30">
         <v>32</v>
@@ -4346,7 +4367,7 @@
         <v>20</v>
       </c>
       <c r="J56" s="31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K56" s="35" t="s">
         <v>69</v>
@@ -4372,7 +4393,7 @@
         <v>153</v>
       </c>
       <c r="T56" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="U56" s="2" t="s">
         <v>154</v>
@@ -5391,19 +5412,7 @@
       <c r="U100" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="P1:P100">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="SI"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="U1:U2"/>
@@ -5419,6 +5428,11 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>